<commit_message>
feat: increased chunk_size and chunk_overlap parameters; feat: adjusted prompt to provide a more balanced response; update: evaluation table and dvc files
</commit_message>
<xml_diff>
--- a/packages/evaluate/gpt4.xlsx
+++ b/packages/evaluate/gpt4.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayyubi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayyubi\Desktop\saadt\the-great-inquirer\packages\evaluate\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="test-1" sheetId="1" r:id="rId1"/>
     <sheet name="test-2" sheetId="2" r:id="rId2"/>
+    <sheet name="test-3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="105">
   <si>
     <t>what is city council doing to address racial inequality?</t>
   </si>
@@ -278,6 +279,78 @@
   </si>
   <si>
     <t>{"card_type": "in_depth", "responses": [{"response": "The transcripts do not provide a direct answer to the question of whether the city council thinks the mayor is doing a good job. However, there are several instances where council members express satisfaction or dissatisfaction with certain aspects of the mayor's actions and decisions. "}, {"response": "For instance, the council expresses appreciation for the mayor's collaboration with the council in passing necessary legislation and ensuring that things were being attended to properly. This suggests that they approve of her efforts in this respect. The council also commends the mayor for working with the civil service to enhance pay for various job classifications, indicating their approval of her efforts to improve the city's economy."}, {"response": "On the other hand, the council expresses concern about the lack of buy-in from the council on certain issues, suggesting that they believe the mayor has not done enough to include them in decision-making processes. They also express dissatisfaction with the way the term \"the city\" is often used to refer to decisions made by the mayor and not the council, indicating that they feel their role in governance is not being adequately recognized."}, {"response": "One of the council members also states that they did not simply rubber-stamp the budget given to them last year, but changed it substantially to reflect council priorities. This could suggest that they were not entirely happy with the original budget proposed by the mayor."}, {"response": "However, without more direct statements from the council members about the mayor's overall performance, it is difficult to definitively say whether they think she is doing a good job. The council's views appear to be mixed, with approval for some of her actions and criticism for others."}], "citations": [{"Title": "Criminal Justice Committee Meeting 4/5/2023", "Published": "4/5/2023", "URL": "https://www.youtube.com/watch?v=CRgme-Yh1yg&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "2:09:46-2:10:11", "Name": "Criminal Justice City Council Meeting Committee Meetings 2023.json"}, {"Title": "Criminal Justice Committee Meeting 4/5/2023", "Published": "4/5/2023", "URL": "https://www.youtube.com/watch?v=CRgme-Yh1yg&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "39:11:00-39:38:00", "Name": "Criminal Justice City Council Meeting Committee Meetings 2023.json"}, {"Title": "City Council Meeting 5/11/2023", "Published": "5/11/2023", "URL": "https://www.youtube.com/watch?v=ZX00_-VUSrM&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "2:36:04-2:36:30", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Criminal Justice Committee Meeting", "Published": "7/12/2023", "URL": "https://www.youtube.com/watch?v=dsO7iShH97E", "Video timestamp": "1:49:17-1:49:45", "Name": "Criminal Justice City Council Meeting Committee Meetings 2023.json"}, {"Title": "City Council Meeting 1/5/23", "Published": "1/5/2023", "URL": "https://www.youtube.com/watch?v=bTR53b05t50&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "1:28:00-1:28:28", "Name": "Regular City Council Meetings 2023.json"}]}</t>
+  </si>
+  <si>
+    <t>describe some successes and failures of city council</t>
+  </si>
+  <si>
+    <t>{"card_type": "in_depth", "responses": [{"response": "Based on the provided transcript, the New Orleans City Council appears to be actively involved in various initiatives to benefit the city and its residents. "}, {"response": "Successes include:"}, {"response": "1. Appropriating grant funds: The council successfully passed an ordinance to appropriate grant funds awarded by FEMA to build resilience in infrastructure and the community. They also approved grants to increase the strength of the public health workforce and for the West Bank Ferry Terminal Renovations planning and construction project."}, {"response": "2. Cooperative Endeavor Agreements: The council authorized the mayor to enter into several cooperative endeavor agreements for the public good, including agreements with the Louisiana Department of Health, the Regional Transit Authority, the Audubon Commission, and Odyssey House Department."}, {"response": "3. Amending city codes and ordinances: The council made amendments to various sections of the city code to clarify language, set performance standards and fees, and adjust the operating budget."}, {"response": "4. Addressing blight: Councilmember Green emphasized the council's focus on reducing blight in the city. "}, {"response": "Failures or challenges:"}, {"response": "1. Deferred decisions: The council deferred the decision on Ordce calendar number 34 265 to a later date, indicating that they perhaps needed more time to come to a consensus on the issue."}, {"response": "2. Mixed public responses: A member of the public acknowledged the council's efforts in promoting affordable units but suggested that there might be room for improvement."}, {"response": "3. Potential lack of effectiveness in certain initiatives: While the council's focus on reducing blight is commendable, Councilmember Green acknowledges that it's a \"very challenging issue,\" suggesting that their efforts may not have been as successful as desired. "}, {"response": "However, it's important to note that the transcript provides limited information and might not fully cover the scope of the question. There might be other successes and failures not mentioned in this council meeting."}], "citations": [{"Title": "City Council Meeting 4/6/2023", "Published": "4/6/2023", "URL": "https://www.youtube.com/watch?v=BdORXbpqGVI&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "2:49:33-2:50:00", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 5/11/2023", "Published": "5/11/2023", "URL": "https://www.youtube.com/watch?v=ZX00_-VUSrM&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "5:41:42-5:42:11", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Regular Council Meeting", "Published": "7/27/2023", "URL": "https://www.youtube.com/watch?v=gSft2c7mAhE", "Video timestamp": "4:30:26-4:30:51", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 3-9-2023", "Published": "3/9/2023", "URL": "https://www.youtube.com/watch?v=qTNPq_Gv5-E&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "5:50:39-5:51:04", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Regular Council Meeting", "Published": "7/27/2023", "URL": "https://www.youtube.com/watch?v=gSft2c7mAhE", "Video timestamp": "3:56:23-3:56:52", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Regular Council Meeting", "Published": "7/27/2023", "URL": "https://www.youtube.com/watch?v=gSft2c7mAhE", "Video timestamp": "3:22:22-3:22:55", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 3-9-2023", "Published": "3/9/2023", "URL": "https://www.youtube.com/watch?v=qTNPq_Gv5-E&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "5:17:00-5:17:27", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Regular Council Meeting", "Published": "7/27/2023", "URL": "https://www.youtube.com/watch?v=gSft2c7mAhE", "Video timestamp": "3:27:13-3:27:40", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 1-19-2023", "Published": "1/19/2023", "URL": "https://www.youtube.com/watch?v=7Nro7f26oEo&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "4:54:43-4:55:10", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Regular Council Meeting", "Published": "7/27/2023", "URL": "https://www.youtube.com/watch?v=gSft2c7mAhE", "Video timestamp": "4:34:56-4:35:20", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 1-19-2023", "Published": "1/19/2023", "URL": "https://www.youtube.com/watch?v=7Nro7f26oEo&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "4:20:25-4:20:53", "Name": "Regular City Council Meetings 2023.json"}]}</t>
+  </si>
+  <si>
+    <t>{"card_type": "in_depth", "responses": [{"response": "The transcripts from the New Orleans city council meeting reveal a number of successes and challenges faced by the council."}, {"response": "One of the main successes highlighted in the transcripts was the council's ability to pass several ordinances and motions. For instance, a motion by council member Harris directing the City Planning Commission to conduct a public hearing to consider amending the text of the comprehensive zoning ordinance to create standards for affordable home ownership opportunities was passed. Additionally, an ordinance authorizing the mayor of the City of New Orleans to enter into a Cooperative Endeavor agreement between the City of New Orleans and Odyssey House was passed. These examples indicate the council's ability to make decisions and push forward legislative actions."}, {"response": "Another success was the council's focus on addressing issues of housing and blight in the city. The council was seen discussing and approving measures related to zoning changes, affordable housing, and penalties for code violations to reduce blight. "}, {"response": "However, the transcripts also reveal some challenges or failures. One of the major issues raised was the potential negative impact of changing zoning from multi-family housing to single-family housing. The speaker argued that this change would limit the amount of housing available to the citizens of New Orleans, which could be viewed as a failure to address housing needs adequately. "}, {"response": "The transcripts also revealed some procedural issues. For example, at one point, a council member suggested temporarily passing over an item and coming back to it later, indicating that the flow of the meeting might not have been as smooth or efficient as it could have been. "}, {"response": "Overall, the transcripts illustrate a council that is actively working to address the city's needs but also facing some challenges in doing so."}], "citations": [{"Title": "City Council Meeting 3-9-2023", "Published": "3/9/2023", "URL": "https://www.youtube.com/watch?v=qTNPq_Gv5-E&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "5:02:45-5:03:15", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 3/23/2023", "Published": "3/23/2023", "URL": "https://www.youtube.com/watch?v=xVZ-oOFqv70&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "7:12:11-7:12:40", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Regular Council Meeting", "Published": "7/27/2023", "URL": "https://www.youtube.com/watch?v=gSft2c7mAhE", "Video timestamp": "3:28:50-3:29:17", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 1-19-2023", "Published": "1/19/2023", "URL": "https://www.youtube.com/watch?v=7Nro7f26oEo&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "3:52:57-3:53:25", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Regular City Council Meeting 4/20/2023", "Published": "4/20/2023", "URL": "https://www.youtube.com/watch?v=TUQ8MxcIWQI&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "4:58:10-4:58:34", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Regular Council Meeting", "Published": "7/27/2023", "URL": "https://www.youtube.com/watch?v=gSft2c7mAhE", "Video timestamp": "3:58:32-3:58:59", "Name": "Regular City Council Meetings 2023.json"}]}</t>
+  </si>
+  <si>
+    <t>{"card_type": "in_depth", "responses": [{"response": "The city council has seen a number of successes and failures, as is evident from the transcripts. "}, {"response": "On the success front, the council has made significant strides in a variety of areas. For instance, they approved an ordinance to amend the operating budget, showcasing their ability to manage the city's finances effectively. They were also able to get a number of motions and resolutions passed, such as the one recognizing the city and its people's belief in human rights. It's also noteworthy that they were able to encourage other taxing authorities to roll back to hold taxes in line for citizens, reflecting their commitment to economic stability. The council also demonstrated its commitment to public safety, with council member Morrell highlighting the urgency of addressing crime and public safety issues. "}, {"response": "However, there have also been some failures. For example, a motion proposed by council members King failed overwhelmingly in the criminal justice committee. This suggests that there can be significant disagreements within the council that can hinder the progress of certain initiatives. A criticism raised by the council member is that there's a lack of urgency in addressing issues of crime and public safety. Also, while the council has taken steps to address public safety issues in the past quarter, it seems that more progress is needed in implementing new initiatives aimed at improving public safety in the community. "}, {"response": "Further, the council seems to struggle with ensuring consistent attendance at meetings. This could potentially impact the efficiency and effectiveness of the council's decision-making process. "}, {"response": "In summary, while the city council has had several successes in passing resolutions and managing the city's budget, it has also faced challenges in areas such as public safety, internal disagreements, and ensuring consistent attendance at meetings."}], "citations": [{"Title": "City Council Meeting 1-19-2023", "Published": "1/19/2023", "URL": "https://www.youtube.com/watch?v=7Nro7f26oEo&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "2:32:00-2:32:23", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 3-9-2023", "Published": "3/9/2023", "URL": "https://www.youtube.com/watch?v=qTNPq_Gv5-E&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "5:06:06-5:06:34", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 5/11/2023", "Published": "5/11/2023", "URL": "https://www.youtube.com/watch?v=ZX00_-VUSrM&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "4:32:40-4:33:14", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Regular City Council Meeting 4/20/2023", "Published": "4/20/2023", "URL": "https://www.youtube.com/watch?v=TUQ8MxcIWQI&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "3:52:45-3:53:11", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 3/23/2023", "Published": "3/23/2023", "URL": "https://www.youtube.com/watch?v=xVZ-oOFqv70&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "6:18:13-6:18:38", "Name": "Regular City Council Meetings 2023.json"}]}</t>
+  </si>
+  <si>
+    <t>{"card_type": "in_depth", "responses": [{"response": "Based on the transcripts, the New Orleans City Council has had a number of successes. For instance, they were able to suspend the rules and adopt an amendment concerning the New Orleans Police Department for a six-month period. The resolution passed without opposition, reflecting unanimity among council members. They also successfully approved the mayor's reappointment of Elizabeth Bowe to the New Orleans criminal justice Council."}, {"response": "The council also passed a motion to add the president of the council as a signatory to a Cooperative Endeavor Agreement between the City of New Orleans and New Orleans Community Day. They managed to pass ordinances to amend budgets of expenditures and to appropriate additional funds to various departments within the city. This included the Department of Public Works and the Department of Workforce Development."}, {"response": "They also successfully authorized the mayor to enter into various Cooperative Endeavor Agreements, including one with the New Orleans Humane Law and Rescue LLC. They managed to amend and reordain sections of the city code to clarify language and penalties for code violations. They also passed a resolution urging the New Orleans Police Department and other city departments to take certain actions."}, {"response": "However, the transcripts also reveal some challenges faced by the council. For instance, one council member expressed frustration that the council was given no opportunity to participate or give input regarding the legal strategy of certain cases. The council member felt that they were limited to receiving briefings and giving opinions, but did not have control over strategy. This could be seen as a failure in terms of the council's ability to influence important legal matters affecting the city."}, {"response": "Another issue that arose was the challenge of reducing blight in the city. While the council has been focused on this issue, it remains a significant problem. A positive note is that there were measures taken to increase hiring rates and annual salaries, but this could also be seen as a challenge in terms of budget allocation and financial management."}, {"response": "In summary, the New Orleans City Council has had a number of successes in passing resolutions, ordinances, and agreements. However, they have also faced challenges in terms of their influence over legal matters, tackling persistent problems like city blight, and managing the city's finances."}], "citations": [{"Title": "City Council Meeting 3/23/2023", "Published": "3/23/2023", "URL": "https://www.youtube.com/watch?v=xVZ-oOFqv70&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "7:25:10-7:25:39", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Regular City Council Meeting 4/20/2023", "Published": "4/20/2023", "URL": "https://www.youtube.com/watch?v=TUQ8MxcIWQI&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "3:49:00-3:49:22", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Regular Council Meeting", "Published": "7/27/2023", "URL": "https://www.youtube.com/watch?v=gSft2c7mAhE", "Video timestamp": "3:58:32-3:58:59", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 1-19-2023", "Published": "1/19/2023", "URL": "https://www.youtube.com/watch?v=7Nro7f26oEo&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "4:20:25-4:20:53", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Criminal Justice Committee Meeting", "Published": "7/12/2023", "URL": "https://www.youtube.com/watch?v=dsO7iShH97E", "Video timestamp": "1:31:18-1:31:42", "Name": "Criminal Justice City Council Meeting Committee Meetings 2023.json"}, {"Title": "Regular City Council Meeting 4/20/2023", "Published": "4/20/2023", "URL": "https://www.youtube.com/watch?v=TUQ8MxcIWQI&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "4:46:19-4:46:57", "Name": "Regular City Council Meetings 2023.json"}]}</t>
+  </si>
+  <si>
+    <t>{"card_type": "in_depth", "responses": [{"response": "Based on the transcripts, the city council has seen a number of successes. For instance, they have passed ordinances to provide an operating budget of expenditures for the City of New Orleans for the year 2023. This includes appropriating funds for rental assistance programs, creating programs to assist homeowners in addressing code enforcement violations, and planning for the historical district landmarks commission. The council has also authorized agreements to utilize American Rescue Plan funds for public purposes such as addressing economic hardship related to the COVID-19 pandemic and providing assistance to constituents with utility arrears. They have also managed to appropriate funds to various departments and projects including the Healthcare for the Homeless program, the Office of Cultural Economy, and the Department of Workforce Development."}, {"response": "In terms of failures, the transcripts do not provide specific examples. However, one could infer a potential challenge from the statement about the ongoing crisis in the city that can no longer be ignored. This statement suggests that there may have been failures in adequately addressing this crisis in a timely manner. The fact that the council did not rubber-stamp the budget they were given, instead choosing to substantially change it, might also indicate dissatisfaction with initial budget proposals. This suggests that there may have been challenges in aligning the council's priorities with those of the mayor's office or other city departments."}, {"response": "Overall, the transcripts highlight the city council's proactive role in managing the city's budget, appropriating funds, and addressing pressing issues. However, they also suggest potential areas of difficulty, including managing crises and aligning priorities among different stakeholders."}], "citations": [{"Title": "City Council Meeting 6/8/2023", "Published": "6/8/2023", "URL": "https://www.youtube.com/watch?v=XDMh4kiWRnM&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "4:31:54-4:32:26", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Regular Council Meeting", "Published": "6/8/2023", "URL": "https://www.youtube.com/watch?v=XDMh4kiWRnM", "Video timestamp": "4:31:54-4:32:26", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 1-19-2023", "Published": "1/19/2023", "URL": "https://www.youtube.com/watch?v=7Nro7f26oEo&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "1:59:08-1:59:31", "Name": "Regular City Council Meetings 2023.json"}]}</t>
+  </si>
+  <si>
+    <t>{"card_type": "in_depth", "responses": [{"response": "Based on the information provided in the transcripts, the council members of New Orleans are:"}, {"response": "1. Council Greene\n2. Council member Morrell\n3. Council member Thomas\n4. Council member Moreno\n5. Council member King\n6. Council member Harris\n7. Council member Jerusal "}, {"response": "Please note that the transcripts do not provide the first names of some council members."}], "citations": [{"Title": "City Council Meeting 3/23/2023", "Published": "3/23/2023", "URL": "https://www.youtube.com/watch?v=xVZ-oOFqv70&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "1:38:45-1:39:11", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 6/8/2023", "Published": "6/8/2023", "URL": "https://www.youtube.com/watch?v=XDMh4kiWRnM&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "4:06:43-4:07:12", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Regular Council Meeting", "Published": "6/8/2023", "URL": "https://www.youtube.com/watch?v=XDMh4kiWRnM", "Video timestamp": "4:06:43-4:07:12", "Name": "Regular City Council Meetings 2023.json"}]}</t>
+  </si>
+  <si>
+    <t>{"card_type": "in_depth", "responses": [{"response": "Based on the transcripts, the council members of the City of New Orleans are:"}, {"response": "1. Council member King\n2. Council member Moreno\n3. Council member Thomas\n4. Council member Jerusalem (this could possibly be a transcription error as there seems to be no council member with this name in New Orleans)\n5. Council member Morrell\n6. Council member Green\n7. Council member Harris"}, {"response": "Please note that the accuracy of this information is based on the provided transcript and may not reflect the current composition of the council."}], "citations": [{"Title": "City Council Meeting 4/6/2023", "Published": "4/6/2023", "URL": "https://www.youtube.com/watch?v=BdORXbpqGVI&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "1:02:41-1:03:16", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 4/6/2023", "Published": "4/6/2023", "URL": "https://www.youtube.com/watch?v=BdORXbpqGVI&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "2:10:22-2:10:51", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 4/6/2023", "Published": "4/6/2023", "URL": "https://www.youtube.com/watch?v=BdORXbpqGVI&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "2:18:36-2:19:04", "Name": "Regular City Council Meetings 2023.json"}]}</t>
+  </si>
+  <si>
+    <t>{"card_type": "in_depth", "responses": [{"response": "The transcripts mention several council members of the New Orleans city council. They are:"}, {"response": "1. Helena Moreno: She is identified as the longest serving consecutive president of the city council and also served with the speaker in the Louisiana legislature."}, {"response": "2. Thomas: He is mentioned in relation to several resolutions, including r236 and or 23 321."}, {"response": "3. Morrell: He is frequently mentioned, including in relation to seconding motions and resolutions. He is also elected to serve as president of the council."}, {"response": "4. Jeruso: He is also mentioned several times, including in seconding motions and resolutions."}, {"response": "5. Harris: He is mentioned in relation to resolution R 23157."}, {"response": "6. King: Mentioned in relation to motion M23 320."}, {"response": "7. Green: He is mentioned in relation to being added as a signatory to a loan agreement."}, {"response": "The transcripts do not provide any further information about these council members, such as their full names or the specifics of their roles within the council beyond what is mentioned in relation to specific motions and resolutions."}], "citations": [{"Title": "City Council Meeting 1/5/23", "Published": "1/5/2023", "URL": "https://www.youtube.com/watch?v=bTR53b05t50&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "1:22:49-1:23:16", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 1/5/23", "Published": "1/5/2023", "URL": "https://www.youtube.com/watch?v=bTR53b05t50&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "3:16:42-3:17:09", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 3-9-2023", "Published": "3/9/2023", "URL": "https://www.youtube.com/watch?v=qTNPq_Gv5-E&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "2:47:28-2:47:59", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Regular City Council Meeting 4/20/2023", "Published": "4/20/2023", "URL": "https://www.youtube.com/watch?v=TUQ8MxcIWQI&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "4:00:08-4:00:40", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Regular Council Meeting", "Published": "7/27/2023", "URL": "https://www.youtube.com/watch?v=gSft2c7mAhE", "Video timestamp": "4:06:28-4:06:58", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 3-9-2023", "Published": "3/9/2023", "URL": "https://www.youtube.com/watch?v=qTNPq_Gv5-E&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "5:15:46-5:16:18", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 4/6/2023", "Published": "4/6/2023", "URL": "https://www.youtube.com/watch?v=BdORXbpqGVI&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "2:49:33-2:50:00", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 3/23/2023", "Published": "3/23/2023", "URL": "https://www.youtube.com/watch?v=xVZ-oOFqv70&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "1:39:16-1:39:41", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Regular City Council Meeting 4/20/2023", "Published": "4/20/2023", "URL": "https://www.youtube.com/watch?v=TUQ8MxcIWQI&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "5:19:19-5:19:44", "Name": "Regular City Council Meetings 2023.json"}]}</t>
+  </si>
+  <si>
+    <t>{"card_type": "in_depth", "responses": [{"response": "The transcript mentions the following city council members: "}, {"response": "1. Councilmember Thomas\n2. Councilmember Green\n3. Councilmember Morrell (referred to as both \"Moran Morrell\" and \"JP Morrell\")\n4. Councilmember Moreno (referred to as both \"Helena Moreno\" and \"Moreno\")\n5. Councilmember King\n6. Councilmember Harris\n7. Councilmember Jerusalem"}, {"response": "These council members appear to be present and active in the council meetings, participating in various discussions, voting, and presenting. Councilmember Moreno is specifically mentioned as the longest serving consecutive president of the city council, and Councilmember Morrell is elected to serve as president with Moreno serving as vice president in the upcoming term."}], "citations": [{"Title": "City Council Meeting 6/8/2023", "Published": "6/8/2023", "URL": "https://www.youtube.com/watch?v=XDMh4kiWRnM&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "1:15:28-1:16:02", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 3-9-2023", "Published": "3/9/2023", "URL": "https://www.youtube.com/watch?v=qTNPq_Gv5-E&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "50:48:00-51:19:00", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 3/23/2023", "Published": "3/23/2023", "URL": "https://www.youtube.com/watch?v=xVZ-oOFqv70&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "4:24:16-4:24:40", "Name": "Regular City Council Meetings 2023.json"}]}</t>
+  </si>
+  <si>
+    <t>{"card_type": "in_depth", "responses": [{"response": "According to the transcript, the New Orleans city council is taking multiple steps to address racial inequality. One of the key areas they are focusing on is housing. Councilman King has requested a zoning change to increase the amount of housing in the city. However, there is a concern that changing from multi-family housing to single-family housing might limit the amount of housing available to the citizens."}, {"response": "The council is also working on economic development and beautification projects in various communities, with a focus on supporting strategic plans. They are allocating resources to these projects through the appropriation of State Act 170 funds awarded to the office of the mayor."}, {"response": "The council also recognizes the need for fairness and inclusivity. They are urging the mayor to conduct a national search for a superintendent of police and engage in a fair, inclusive, transparent, and clearly defined public process for the selection."}, {"response": "Council members are also encouraging minority business owners and have shown support for them in the community. They are working with the collaborative, a group that supports minority business owners."}, {"response": "Another initiative involves the appropriation of unspent grant funds to the Department of Workforce Development. This suggests an effort to improve employment opportunities, which could play a role in addressing racial inequality."}, {"response": "Lastly, the council is reaffirming its commitment to the quality and safety of all, including transgender and gender non-conforming individuals. They recognize the inherent human rights to equal opportunity and a safe environment within all institutions."}, {"response": "In conclusion, the New Orleans city council is taking a multi-pronged approach to address racial inequality, focusing on areas such as housing, economic development, police leadership, support for minority businesses, workforce development, and human rights."}], "citations": [{"Title": "City Council Meeting 3/23/2023", "Published": "3/23/2023", "URL": "https://www.youtube.com/watch?v=xVZ-oOFqv70&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "6:12:01-6:12:22", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Regular City Council Meeting 4/20/2023", "Published": "4/20/2023", "URL": "https://www.youtube.com/watch?v=TUQ8MxcIWQI&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "3:48:30-3:48:53", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 2-2-2023", "Published": "2/2/2023", "URL": "https://www.youtube.com/watch?v=Bl-Tv5yuUTw&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "3:37:59-3:38:24", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 1-19-2023", "Published": "1/19/2023", "URL": "https://www.youtube.com/watch?v=7Nro7f26oEo&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "4:26:59-4:27:23", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 6/8/2023", "Published": "6/8/2023", "URL": "https://www.youtube.com/watch?v=XDMh4kiWRnM&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "1:32:37-1:33:00", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Regular Council Meeting", "Published": "6/8/2023", "URL": "https://www.youtube.com/watch?v=XDMh4kiWRnM", "Video timestamp": "1:32:37-1:33:00", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 6/8/2023", "Published": "6/8/2023", "URL": "https://www.youtube.com/watch?v=XDMh4kiWRnM&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "4:19:05-4:19:32", "Name": "Regular City Council Meetings 2023.json"}]}</t>
+  </si>
+  <si>
+    <t>{"card_type": "in_depth", "responses": [{"response": "Based on the transcripts, the New Orleans City Council is addressing racial inequality through several measures. "}, {"response": "Firstly, it is focusing on affordable housing, which is a significant issue that disproportionately affects racial minorities. The City Council is united in its goal to provide affordable housing in New Orleans and has taken measures to create more homeowners, as seen in the motion M 2322 and other initiatives. This is seen as a way to build wealth and long-term stability in the city, thus addressing the wealth gap that is often along racial lines."}, {"response": "Secondly, the City Council is also striving for equal opportunity and safety for all, including transgender and gender non-conforming individuals, through the resolution R 23 199. This resolution reaffirms the City Council's commitment to human rights and the safety of diverse groups, including those diverse in their sexuality and gender identities and expressions."}, {"response": "Thirdly, the City Council is advocating for justice and addressing discriminatory practices. While the transcripts don't provide specific actions, it is clear Council members are actively involved in advocating for the citizens of the city and are committed to addressing and resolving issues of discrimination. "}, {"response": "Lastly, the City Council is proactive in encouraging local citizens to fill various job classifications to enhance pay where necessary. This can help to address income inequality, a factor that often intersects with racial inequality."}, {"response": "However, the transcripts do not provide a comprehensive overview of all the measures taken by the City Council to address racial inequality."}], "citations": [{"Title": "City Council Meeting 1-19-2023", "Published": "1/19/2023", "URL": "https://www.youtube.com/watch?v=7Nro7f26oEo&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "4:40:59-4:41:30", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 5/11/2023", "Published": "5/11/2023", "URL": "https://www.youtube.com/watch?v=ZX00_-VUSrM&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "5:28:16-5:28:43", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Regular Council Meeting", "Published": "7/27/2023", "URL": "https://www.youtube.com/watch?v=gSft2c7mAhE", "Video timestamp": "3:21:20-3:21:46", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 3/23/2023", "Published": "3/23/2023", "URL": "https://www.youtube.com/watch?v=xVZ-oOFqv70&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "6:09:50-6:10:15", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 6/8/2023", "Published": "6/8/2023", "URL": "https://www.youtube.com/watch?v=XDMh4kiWRnM&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "4:19:05-4:19:32", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Regular Council Meeting", "Published": "6/8/2023", "URL": "https://www.youtube.com/watch?v=XDMh4kiWRnM", "Video timestamp": "4:19:05-4:19:32", "Name": "Regular City Council Meetings 2023.json"}]}</t>
+  </si>
+  <si>
+    <t>{"card_type": "in_depth", "responses": [{"response": "Based on the transcripts, the New Orleans City Council is taking several measures to address racial inequality. "}, {"response": "1. Economic Development: The council has authorized the mayor to enter into a Cooperative Endeavor agreement with Greater New Orleans Inc for promoting economic growth and prosperity for all its citizens, which could potentially address economic disparities often tied to racial inequality."}, {"response": "2. Technology Access: The council has appropriated grant funds to purchase computers and virtual reality headsets for virtual reality training, possibly helping to bridge the digital divide which disproportionately affects racial minorities."}, {"response": "3. Public Defender's Office: The council has appropriated funds to The Orleans Parish Public Defender's office for representation to indigent persons accused of crimes. This could potentially address racial disparities in the criminal justice system."}, {"response": "4. Rental Assistance Programs: The council is appropriating funds for rental assistance programs in the Office of Community Development. This might help address housing instability which disproportionately affects people of color."}, {"response": "5. Broadband Outreach: The council has appropriated funds awarded by the Federal Communications Commission to the Office of Resilience and Sustainability for the New Orleans Broadband Outreach, which could help address the digital divide."}, {"response": "6. Community Engagement: The council is urging the Mayor to conduct a national search for a new police superintendent with a fair, inclusive, transparent, and clearly defined public process that includes community engagement. This could potentially address issues of trust and representation between law enforcement and racially diverse communities."}, {"response": "7. Addressing Institutional Racist Policies: A council member suggested undoing institutional racist policies passed after Hurricane Katrina, which he claims negatively impact children and their parents. "}, {"response": "It should be noted that while these initiatives have the potential to address racial inequality, the transcripts do not provide explicit confirmation that they are targeted specifically at racial inequality, or detail about their effectiveness."}], "citations": [{"Title": "City Council Meeting 6/8/2023", "Published": "6/8/2023", "URL": "https://www.youtube.com/watch?v=XDMh4kiWRnM&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "4:35:47-4:36:16", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Regular Council Meeting", "Published": "6/8/2023", "URL": "https://www.youtube.com/watch?v=XDMh4kiWRnM", "Video timestamp": "4:35:47-4:36:16", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 1-19-2023", "Published": "1/19/2023", "URL": "https://www.youtube.com/watch?v=7Nro7f26oEo&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "4:54:43-4:55:10", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Regular Council Meeting", "Published": "7/13/2023", "URL": "https://www.youtube.com/watch?v=39kWL1P9NoI", "Video timestamp": "3:00:33-3:00:57", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 3/23/2023", "Published": "3/23/2023", "URL": "https://www.youtube.com/watch?v=xVZ-oOFqv70&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "2:45:42-2:46:09", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 6/8/2023", "Published": "6/8/2023", "URL": "https://www.youtube.com/watch?v=XDMh4kiWRnM&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "4:36:57-4:37:22", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 4/6/2023", "Published": "4/6/2023", "URL": "https://www.youtube.com/watch?v=BdORXbpqGVI&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "2:49:33-2:50:00", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 5/11/2023", "Published": "5/11/2023", "URL": "https://www.youtube.com/watch?v=ZX00_-VUSrM&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "4:34:05-4:34:30", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Regular Council Meeting", "Published": "7/27/2023", "URL": "https://www.youtube.com/watch?v=gSft2c7mAhE", "Video timestamp": "4:39:08-4:39:36", "Name": "Regular City Council Meetings 2023.json"}]}</t>
+  </si>
+  <si>
+    <t>{"card_type": "in_depth", "responses": [{"response": "The New Orleans City Council is addressing racial inequality through various initiatives and policies as per the provided transcripts. Council Member Jerusalem Moreno Green is focusing on economic development by proposing amendments to allocate unspent funds to the Department of Workforce Development. This initiative is aimed at promoting economic growth and opportunities, which could provide minority business owners with greater opportunities."}, {"response": "The Council is also working on issues of affordable housing and gentrification, which disproportionately affect minority populations. Council members are seeking to work collaboratively to achieve victories in housing affordability, which is a crucial aspect of addressing racial inequalities."}, {"response": "Additionally, the City Council is involved in tackling institutional racist policies. One speaker suggested the solution to juvenile crime in New Orleans lies in undoing such policies enacted post-Hurricane Katrina, which have negatively impacted children and their parents. The Council also supports initiatives that challenge capitalist domination of New Orleans schools and advocate for an education system that teaches children about their true history and role in society."}, {"response": "Furthermore, the Council is addressing racial inequality by issuing resolutions that reaffirm its commitment to the safety and equality of all individuals, including those diverse in their sexuality and gender identities. "}, {"response": "The Council is also working to address homelessness, which disproportionately affects minority communities. They've partnered with Clutch Consulting Group to build an office that aims to create sustainable changes for the city's homeless population. "}, {"response": "In conclusion, the New Orleans City Council is addressing racial inequality through a variety of measures that focus on economic development, housing affordability, education, and law enforcement strategies. They also strive to foster an inclusive and safe environment for all citizens, irrespective of their race, gender, or sexual orientation."}], "citations": [{"Title": "Regular City Council Meeting 4/20/2023", "Published": "4/20/2023", "URL": "https://www.youtube.com/watch?v=TUQ8MxcIWQI&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "5:19:19-5:19:44", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Regular Council Meeting", "Published": "7/27/2023", "URL": "https://www.youtube.com/watch?v=gSft2c7mAhE", "Video timestamp": "4:34:56-4:35:20", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 3-9-2023", "Published": "3/9/2023", "URL": "https://www.youtube.com/watch?v=qTNPq_Gv5-E&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "2:41:14-2:41:44", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Criminal Justice Committee Meeting 5/10/2023", "Published": "5/10/2023", "URL": "https://www.youtube.com/watch?v=kqfTCmIlvjw&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "2:12:50-2:13:14", "Name": "Criminal Justice City Council Meeting Committee Meetings 2023.json"}, {"Title": "City Council Meeting 1/5/23", "Published": "1/5/2023", "URL": "https://www.youtube.com/watch?v=bTR53b05t50&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "2:39:24-2:39:50", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Regular Council Meeting", "Published": "7/27/2023", "URL": "https://www.youtube.com/watch?v=gSft2c7mAhE", "Video timestamp": "3:53:11-3:53:39", "Name": "Regular City Council Meetings 2023.json"}]}</t>
+  </si>
+  <si>
+    <t>{"card_type": "in_depth", "responses": [{"response": "The transcripts provide some insights into how the city council is addressing racial inequality. They are passing and recommending approval for several resolutions and motions to address various aspects of racial and social inequality. For instance, the resolution R23 255 by council members Moreno, Morrell, Jeruso, Harris, King, Green, and Thomas recommended by the climate change and sustainability committee appears to be part of the consent agenda, however, the exact details of this resolution in addressing racial inequality are not explicitly mentioned in the transcript."}, {"response": "Another resolution, R23 343, reaffirms the council's commitment to the quality and safety of all, including transgender and gender non-conforming individuals. This resolution emphasizes that all individuals, regardless of their sexuality and gender identities, have the inherent human rights to equal opportunity and a safe environment within all institutions. This resolution seems to be a step towards addressing inequality based on gender identity and expression."}, {"response": "The city council also passed resolution R 23 199, recognizing the city's commitment to human rights, especially for the most vulnerable communities. Council members expressed hope that the resolution would encourage legislators from around the state to do the right thing, signaling an intention to influence broader policy change to address inequality."}, {"response": "Furthermore, the council is urging the mayor of New Orleans to conduct a fair, inclusive, and transparent search process for the new superintendent of police, which could suggest an attempt to address racial inequality in law enforcement."}, {"response": "Lastly, the council ratified the appointment of council members to the New Orleans Civil Service Commission. This could potentially address racial inequality if the appointed members are committed to promoting diversity and equity in civil service."}, {"response": "In summary, while the transcripts do not provide specific details on the strategies or policies the city council is implementing to address racial inequality, it does indicate that the city council is actively passing resolutions and taking steps to promote fairness, inclusivity, and human rights."}], "citations": [{"Title": "Regular Council Meeting", "Published": "6/8/2023", "URL": "https://www.youtube.com/watch?v=XDMh4kiWRnM", "Video timestamp": "1:24:02-1:24:39", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 6/8/2023", "Published": "6/8/2023", "URL": "https://www.youtube.com/watch?v=XDMh4kiWRnM&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "4:08:18-4:08:45", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Regular Council Meeting", "Published": "6/8/2023", "URL": "https://www.youtube.com/watch?v=XDMh4kiWRnM", "Video timestamp": "4:08:18-4:08:45", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Regular Council Meeting", "Published": "6/8/2023", "URL": "https://www.youtube.com/watch?v=XDMh4kiWRnM", "Video timestamp": "1:23:27-1:23:56", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 6/8/2023", "Published": "6/8/2023", "URL": "https://www.youtube.com/watch?v=XDMh4kiWRnM&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "1:23:27-1:23:56", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Regular City Council Meeting 4/20/2023", "Published": "4/20/2023", "URL": "https://www.youtube.com/watch?v=TUQ8MxcIWQI&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "2:59:47-3:00:11", "Name": "Regular City Council Meetings 2023.json"}]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"card_type": "in_depth", "responses": [{"response": "A proviso, as mentioned in the transcripts, refers to a condition or stipulation that is attached to an agreement, decision, or ordinance. In the context of the New Orleans city council meeting, it appears that provisos are being used as conditions or requirements that must be met in the implementation of a motion, ordinance, or zoning request. For example, in the case of a conditional use request on zoning docket 423, it was granted subject to a proviso stated in the city planning commission's report. In another instance, an ordinance was subject to eight provisos set forward in the city planning commission's staff report along with two additional provisos. These included requirements for the applicant to comply with certain standards for building design and yard regulations. In summary, a proviso functions as a condition or requirement that must be fulfilled for an agreement, decision, or ordinance to be fully implemented or approved."}], "citations": [{"Title": "Regular Council Meeting", "Published": "7/27/2023", "URL": "https://www.youtube.com/watch?v=gSft2c7mAhE", "Video timestamp": "3:27:13-3:27:40", "Name": "Regular City Council Meetings 2023.json"}]}  </t>
+  </si>
+  <si>
+    <t>{"card_type": "in_depth", "responses": [{"response": "A proviso, as mentioned in the transcripts, refers to a condition or stipulation that is set forth in a legislation or official document. In the context of the New Orleans city council meeting, provisos are used as conditional terms or requirements that need to be met in various contexts. For example, the transcripts mention provisos set forward by the city planning commission's staff report that must be complied with by applicants. These include compliance with certain standards for bulk and yard regulations, as well as specific building design standards for historic urban neighborhoods. Provisos can also be used to limit or regulate certain activities or operations, as mentioned in the case where events are recommended to occur only when the school is not in session. Overall, provisos are terms or conditions that must be met in order to achieve compliance with a specific legislation, agreement, or official document."}], "citations": [{"Title": "City Council Meeting 3/23/2023", "Published": "3/23/2023", "URL": "https://www.youtube.com/watch?v=xVZ-oOFqv70&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "6:48:00-6:48:28", "Name": "Regular City Council Meetings 2023.json"}]}</t>
+  </si>
+  <si>
+    <t>{"card_type": "in_depth", "responses": [{"response": "An ordinance, in the context of the New Orleans City Council, is a piece of legislation or law enacted by the city council to govern or regulate various aspects of the city's operations and residents' behavior. It is a formal rule or law that the city government makes to regulate public affairs. "}, {"response": "The transcripts reference several instances of ordinances being used for different purposes:"}, {"response": "1. Zoning and Planning: The council worked on ordinances related to zoning, such as establishing an interim zoning district for commercial short-term rental. These ordinances can amend existing zoning laws and are typically used to govern land use within the city."}, {"response": "2. Budgetary and Financial Decisions: Ordinances are used to provide operating budgets of revenues and expenditures for the city. They can appropriate funds for specific programs such as rental assistance programs or code enforcement units."}, {"response": "3. Regulatory Purposes: The council discusses ordinances that regulate behaviors such as the possession of firearms in certain zones. Penalties and fees for violations may also be established by ordinances."}, {"response": "4. Contract Approvals: The council uses ordinances to approve contracts and settlements that are required by the council as a matter of law."}, {"response": "5. Enforcement: The council discusses ordinances related to enforcement, such as penalties for illegal dumping and the empowerment of vehicles involved in illegal activities."}, {"response": "The process of passing an ordinance typically involves drafting the legislation, presenting it for a council vote, and, if passed, it becomes legally binding. Amendments to ordinances can also be proposed and passed through a similar process."}], "citations": [{"Title": "City Council Meeting 6/8/2023", "Published": "6/8/2023", "URL": "https://www.youtube.com/watch?v=XDMh4kiWRnM&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "3:51:31-3:51:57", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 1-19-2023", "Published": "1/19/2023", "URL": "https://www.youtube.com/watch?v=7Nro7f26oEo&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "4:22:41-4:23:07", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Regular Council Meeting", "Published": "7/27/2023", "URL": "https://www.youtube.com/watch?v=gSft2c7mAhE", "Video timestamp": "3:47:52-3:48:15", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 2-2-2023", "Published": "2/2/2023", "URL": "https://www.youtube.com/watch?v=Bl-Tv5yuUTw&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "2:26:07-2:26:31", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 2-2-2023", "Published": "2/2/2023", "URL": "https://www.youtube.com/watch?v=Bl-Tv5yuUTw&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "2:08:45-2:09:13", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Regular Council Meeting", "Published": "7/27/2023", "URL": "https://www.youtube.com/watch?v=gSft2c7mAhE", "Video timestamp": "3:27:13-3:27:40", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 6/8/2023", "Published": "6/8/2023", "URL": "https://www.youtube.com/watch?v=XDMh4kiWRnM&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "4:31:54-4:32:26", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Regular Council Meeting", "Published": "6/8/2023", "URL": "https://www.youtube.com/watch?v=XDMh4kiWRnM", "Video timestamp": "4:31:54-4:32:26", "Name": "Regular City Council Meetings 2023.json"}]}</t>
+  </si>
+  <si>
+    <t>{"card_type": "in_depth", "responses": [{"response": "An ordinance, as referred to in these transcripts, is a piece of legislation enacted by a municipal authority, in this case, the City Council of New Orleans. These ordinances cover a wide range of topics and serve various purposes. They can establish or amend sections of the city's code, like increasing penalties for code violations or establishing firearm-free zones. They can also authorize the mayor to enter into cooperative endeavor agreements with various entities, such as the Louisiana Department of Health or the Regional Transit Authority, and provide funds for various city departments and programs. Ordinances can also modify existing agreements, set forth expectations for the law department's communication with the council, and set exemptions for certain contracts. They can be subject to amendments proposed by council members. It's also noted that some sections of an ordinance can be declared invalid without affecting the remaining sections. Overall, ordinances are a key tool for local governments to manage and regulate various aspects of city life."}], "citations": [{"Title": "City Council Meeting 1-19-2023", "Published": "1/19/2023", "URL": "https://www.youtube.com/watch?v=7Nro7f26oEo&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "5:04:42-5:05:08", "Name": "Regular City Council Meetings 2023.json"}]}</t>
+  </si>
+  <si>
+    <t>{"card_type": "in_depth", "responses": [{"response": "Based on the available information in the transcripts, the effectiveness of facial recognition technology used by the New Orleans Police Department (NOPD) is not explicitly clear. On one hand, the NOPD has made efforts to incorporate this technology into their operations as part of their strategic crime plan. They have also initiated a process of producing quarterly data on its use, which indicates a commitment to transparency and accountability."}, {"response": "However, the specific results or impact of using facial recognition technology are not straightforward. For instance, in the fourth quarter of one year, there were six requests for facial recognition, but it is not clear how many of these requests led to successful identifications or arrests. In the first quarter of 2023, there were five facial recognition requests, one was not approved, and though there was one match, it did not result in an arrest. This suggests that the technology may not have been as immediately effective as anticipated."}, {"response": "Moreover, there are also concerns raised in the transcripts about the potential for discriminatory practices in the way the NOPD is policing, and the use of facial recognition technology could potentially contribute to this issue. "}, {"response": "The use of facial recognition technology by law enforcement is a complex issue that involves balancing the potential benefits for crime prevention and solving with concerns about civil liberties, privacy, and the potential for misuse or abuse. Based on the information provided in the transcripts, it seems that the NOPD is in the early stages of using this technology, and further data and analysis would be necessary to fully assess its effectiveness."}], "citations": [{"Title": "Criminal Justice Committee Meeting 5/10/2023", "Published": "5/10/2023", "URL": "https://www.youtube.com/watch?v=kqfTCmIlvjw&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "2:12:50-2:13:14", "Name": "Criminal Justice City Council Meeting Committee Meetings 2023.json"}, {"Title": "Criminal Justice Committee Meeting", "Published": "2/7/2023", "URL": "https://www.youtube.com/watch?v=PwiJYkLNzZA&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "2:49:59-2:50:24", "Name": "Criminal Justice City Council Meeting Committee Meetings 2023.json"}, {"Title": "Criminal Justice Committee Meeting 5/10/2023", "Published": "5/10/2023", "URL": "https://www.youtube.com/watch?v=kqfTCmIlvjw&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "1:04:33-1:04:58", "Name": "Criminal Justice City Council Meeting Committee Meetings 2023.json"}, {"Title": "Criminal Justice Committee Meeting 4/5/2023", "Published": "4/5/2023", "URL": "https://www.youtube.com/watch?v=CRgme-Yh1yg&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "1:48:43-1:49:09", "Name": "Criminal Justice City Council Meeting Committee Meetings 2023.json"}]}</t>
+  </si>
+  <si>
+    <t>{"card_type": "in_depth", "responses": [{"response": "The effectiveness of the New Orleans Police Department's (NOPD) use of facial recognition technology is not definitively established based on the council transcripts. The transcripts highlight that the NOPD has only recently started using facial recognition technology, and it was used in a limited capacity during the initial period. "}, {"response": "In the first quarter of 2023, NOPD made five facial recognition requests with one match but no resulting arrests. In the fourth quarter, six requests were made. However, the details of any matches or arrests from these requests during this quarter are not explicitly mentioned in the transcripts. "}, {"response": "Council members expressed differing views on the technology. While some council members highlighted the importance of having safeguards in place to prevent abuse, others questioned the efficacy of the technology given the absence of proof that it has significantly contributed to solving crimes. "}, {"response": "It was noted that the technology is used as a last resort and that there are safeguards in place to prevent misuse. More than one individual is involved in the decision to utilize facial recognition, and it is not solely in the hands of an individual officer on the street. "}, {"response": "In conclusion, based on the available data from the transcripts, it is not possible to definitively determine the effectiveness of NOPD's use of facial recognition technology. The limited use and lack of detailed outcomes of the requests made so far suggest that further data and analysis would be needed to make a comprehensive assessment."}], "citations": [{"Title": "City Council Meeting 3/23/2023", "Published": "3/23/2023", "URL": "https://www.youtube.com/watch?v=xVZ-oOFqv70&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "7:25:10-7:25:39", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 5/11/2023", "Published": "5/11/2023", "URL": "https://www.youtube.com/watch?v=ZX00_-VUSrM&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "5:29:18-5:29:43", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Criminal Justice Committee Meeting", "Published": "2/7/2023", "URL": "https://www.youtube.com/watch?v=PwiJYkLNzZA&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "2:56:05-2:56:28", "Name": "Criminal Justice City Council Meeting Committee Meetings 2023.json"}, {"Title": "CRIMINAL JUSTICE COMMITTEE 1/23/2023", "Published": "1/23/2023", "URL": "https://www.youtube.com/watch?v=ABsfv6bzOBA&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "2:36:21-2:36:48", "Name": "Criminal Justice City Council Meeting Committee Meetings 2023.json"}, {"Title": "City Council Meeting 1/5/23", "Published": "1/5/2023", "URL": "https://www.youtube.com/watch?v=bTR53b05t50&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "2:49:19-2:49:43", "Name": "Regular City Council Meetings 2023.json"}]}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{"card_type": "in_depth", "responses": [{"response": "Based on the available transcripts, there isn't a clear consensus or explicit statements regarding whether the city council members believe the mayor is doing a good job. However, there are several instances where council members express recognition and appreciation for the mayor's actions and initiatives. "}, {"response": "For example, Council Member Harris commends the mayor for good news at the start of a meeting and Council Member Morrell expresses gratitude for the mayor's support. Council Member Harris also mentions the good work of the mayor in tandem with the council and suggests that this collaborative work has helped to put important things in motion. This could be interpreted as a positive evaluation of the mayor's performance. "}, {"response": "Moreover, the council members have been actively participating in the task force meetings initiated by the mayor. This suggests they are supportive of the mayor's initiatives and are willing to work together to achieve common goals. "}, {"response": "However, it's worth noting that these interpretations are based on the available transcripts and the specific question of whether the city council thinks the mayor is doing a good job is not directly addressed. Therefore, while there are positive interactions and collaborative efforts between the city council and the mayor, a comprehensive assessment of the council's view on the mayor's performance cannot be definitively determined from the provided information."}], "citations": [{"Title": "Regular Council Meeting", "Published": "7/27/2023", "URL": "https://www.youtube.com/watch?v=gSft2c7mAhE", "Video timestamp": "3:22:22-3:22:55", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Regular Council Meeting", "Published": "7/13/2023", "URL": "https://www.youtube.com/watch?v=39kWL1P9NoI", "Video timestamp": "3:19:59-3:20:27", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 4/6/2023", "Published": "4/6/2023", "URL": "https://www.youtube.com/watch?v=BdORXbpqGVI&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "2:29:03-2:29:31", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 1-19-2023", "Published": "1/19/2023", "URL": "https://www.youtube.com/watch?v=7Nro7f26oEo&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "4:40:59-4:41:30", "Name": "Regular City Council Meetings 2023.json"}]} </t>
+  </si>
+  <si>
+    <t>{"card_type": "in_depth", "responses": [{"response": "Based on the transcripts provided, it appears that the city council acknowledges the mayor's efforts and has a working relationship with her. Council members mentioned the mayor's role in legislation and other initiatives, noting that she has worked in tandem with the council. For instance, the mayor was commended for working with the city council to get the necessary legislation put in motion. This effort was appreciated as it was seen as a step towards ensuring that things are attended to properly. "}, {"response": "However, the transcripts also show that council members have been proactive, and they seem to focus on their own initiatives and responsibilities, such as job classifications, budget approvals, and zoning matters. They've also requested that the Civil Service Commission look at various job classifications and enhance pay where necessary. "}, {"response": "Council members also participated in discussions about the mayor's initiatives, such as a cooperative endeavor agreement and the mayor's response to a question about council participation in a meeting. This shows that they are engaged with the mayor's work, but it does not necessarily indicate approval or disapproval of her performance."}, {"response": "In conclusion, while there are no explicit statements of approval or disapproval of the mayor's performance, the council members' comments suggest a collaborative relationship with the mayor."}], "citations": [{"Title": "City Council Meeting 5/11/2023", "Published": "5/11/2023", "URL": "https://www.youtube.com/watch?v=ZX00_-VUSrM&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "2:36:04-2:36:30", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 5/11/2023", "Published": "5/11/2023", "URL": "https://www.youtube.com/watch?v=ZX00_-VUSrM&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "2:32:35-2:33:00", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 6/8/2023", "Published": "6/8/2023", "URL": "https://www.youtube.com/watch?v=XDMh4kiWRnM&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "3:16:58-3:17:27", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Regular Council Meeting", "Published": "6/8/2023", "URL": "https://www.youtube.com/watch?v=XDMh4kiWRnM", "Video timestamp": "3:16:58-3:17:27", "Name": "Regular City Council Meetings 2023.json"}]}</t>
+  </si>
+  <si>
+    <t>{"card_type": "in_depth", "responses": [{"response": "The transcripts show a complex picture of the New Orleans City Council's attitude towards the Mayor. There are instances of collaboration and support but also frustration and criticism."}, {"response": "On one hand, the council members acknowledge the Mayor's efforts. They mention his collaboration with the council to pass necessary legislation and his initiative to involve the council in task force meetings. The council also supports the Mayor's actions by approving ordinances that authorize him to enter into cooperative endeavor agreements with different agencies."}, {"response": "However, the transcripts also show instances of frustration with the Mayor's office. Members express dissatisfaction with the lack of clear leadership and communication from the administration, especially regarding city planning. They express frustration that the council was not involved in decisions that put the city's finances at risk. They also note that the council was not given an opportunity to participate or provide input regarding the legal strategy of some cases."}, {"response": "Overall, the transcripts show that while the council acknowledges the efforts of the Mayor, they also express frustration at times. There are instances of collaboration and support, but also a desire for better communication and inclusion in decision-making processes. However, the transcripts do not provide a clear consensus on whether the council thinks the Mayor is doing a good job."}], "citations": [{"Title": "City Council Meeting 1/5/23", "Published": "1/5/2023", "URL": "https://www.youtube.com/watch?v=bTR53b05t50&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "1:28:00-1:28:28", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 2-2-2023", "Published": "2/2/2023", "URL": "https://www.youtube.com/watch?v=Bl-Tv5yuUTw&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "3:37:59-3:38:24", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 1/5/23", "Published": "1/5/2023", "URL": "https://www.youtube.com/watch?v=bTR53b05t50&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "1:57:59-1:58:30", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 5/11/2023", "Published": "5/11/2023", "URL": "https://www.youtube.com/watch?v=ZX00_-VUSrM&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "5:02:12-5:02:39", "Name": "Regular City Council Meetings 2023.json"}]}</t>
   </si>
 </sst>
 </file>
@@ -645,7 +718,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F10" sqref="A1:O26"/>
     </sheetView>
   </sheetViews>
@@ -1886,8 +1959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection sqref="A1:O31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3353,4 +3426,1567 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O36"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="O33" sqref="O33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2">
+        <v>20</v>
+      </c>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="3"/>
+    </row>
+    <row r="3" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2">
+        <v>20</v>
+      </c>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="3"/>
+    </row>
+    <row r="4" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2">
+        <v>20</v>
+      </c>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="3"/>
+    </row>
+    <row r="5" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2">
+        <v>20</v>
+      </c>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="3"/>
+    </row>
+    <row r="6" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2">
+        <v>20</v>
+      </c>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="3"/>
+    </row>
+    <row r="7" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="4">
+        <v>12000</v>
+      </c>
+      <c r="E7" s="4">
+        <v>6000</v>
+      </c>
+      <c r="F7" s="4">
+        <v>12000</v>
+      </c>
+      <c r="G7" s="4">
+        <v>6000</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L7" s="2">
+        <v>20</v>
+      </c>
+      <c r="M7" s="4">
+        <v>0</v>
+      </c>
+      <c r="N7" s="4">
+        <v>0</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="4">
+        <v>12000</v>
+      </c>
+      <c r="E8" s="4">
+        <v>6000</v>
+      </c>
+      <c r="F8" s="4">
+        <v>12000</v>
+      </c>
+      <c r="G8" s="4">
+        <v>6000</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L8" s="2">
+        <v>20</v>
+      </c>
+      <c r="M8" s="4">
+        <v>0</v>
+      </c>
+      <c r="N8" s="4">
+        <v>1</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="4">
+        <v>12000</v>
+      </c>
+      <c r="E9" s="4">
+        <v>6000</v>
+      </c>
+      <c r="F9" s="4">
+        <v>12000</v>
+      </c>
+      <c r="G9" s="4">
+        <v>6000</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L9" s="2">
+        <v>20</v>
+      </c>
+      <c r="M9" s="4">
+        <v>0</v>
+      </c>
+      <c r="N9" s="4">
+        <v>2</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="4">
+        <v>12000</v>
+      </c>
+      <c r="E10" s="4">
+        <v>6000</v>
+      </c>
+      <c r="F10" s="4">
+        <v>12000</v>
+      </c>
+      <c r="G10" s="4">
+        <v>6000</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L10" s="2">
+        <v>20</v>
+      </c>
+      <c r="M10" s="4">
+        <v>0</v>
+      </c>
+      <c r="N10" s="4">
+        <v>3</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="4">
+        <v>12000</v>
+      </c>
+      <c r="E11" s="4">
+        <v>6000</v>
+      </c>
+      <c r="F11" s="4">
+        <v>12000</v>
+      </c>
+      <c r="G11" s="4">
+        <v>6000</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L11" s="2">
+        <v>20</v>
+      </c>
+      <c r="M11" s="4">
+        <v>0</v>
+      </c>
+      <c r="N11" s="4">
+        <v>4</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="4">
+        <v>12000</v>
+      </c>
+      <c r="E12" s="4">
+        <v>6000</v>
+      </c>
+      <c r="F12" s="4">
+        <v>12000</v>
+      </c>
+      <c r="G12" s="4">
+        <v>6000</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L12" s="2">
+        <v>20</v>
+      </c>
+      <c r="M12" s="4">
+        <v>0</v>
+      </c>
+      <c r="N12" s="4">
+        <v>0</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="4">
+        <v>12000</v>
+      </c>
+      <c r="E13" s="4">
+        <v>6000</v>
+      </c>
+      <c r="F13" s="4">
+        <v>12000</v>
+      </c>
+      <c r="G13" s="4">
+        <v>6000</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L13" s="2">
+        <v>20</v>
+      </c>
+      <c r="M13" s="4">
+        <v>0</v>
+      </c>
+      <c r="N13" s="4">
+        <v>1</v>
+      </c>
+      <c r="O13" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="4">
+        <v>12000</v>
+      </c>
+      <c r="E14" s="4">
+        <v>6000</v>
+      </c>
+      <c r="F14" s="4">
+        <v>12000</v>
+      </c>
+      <c r="G14" s="4">
+        <v>6000</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L14" s="2">
+        <v>20</v>
+      </c>
+      <c r="M14" s="4">
+        <v>0</v>
+      </c>
+      <c r="N14" s="4">
+        <v>2</v>
+      </c>
+      <c r="O14" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="4">
+        <v>12000</v>
+      </c>
+      <c r="E15" s="4">
+        <v>6000</v>
+      </c>
+      <c r="F15" s="4">
+        <v>12000</v>
+      </c>
+      <c r="G15" s="4">
+        <v>6000</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L15" s="2">
+        <v>20</v>
+      </c>
+      <c r="M15" s="4">
+        <v>0</v>
+      </c>
+      <c r="N15" s="4">
+        <v>3</v>
+      </c>
+      <c r="O15" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="4">
+        <v>12000</v>
+      </c>
+      <c r="E16" s="4">
+        <v>6000</v>
+      </c>
+      <c r="F16" s="4">
+        <v>12000</v>
+      </c>
+      <c r="G16" s="4">
+        <v>6000</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L16" s="2">
+        <v>20</v>
+      </c>
+      <c r="M16" s="4">
+        <v>0</v>
+      </c>
+      <c r="N16" s="4">
+        <v>4</v>
+      </c>
+      <c r="O16" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="4">
+        <v>12000</v>
+      </c>
+      <c r="E17" s="4">
+        <v>6000</v>
+      </c>
+      <c r="F17" s="4">
+        <v>12000</v>
+      </c>
+      <c r="G17" s="4">
+        <v>6000</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L17" s="2">
+        <v>20</v>
+      </c>
+      <c r="M17" s="4">
+        <v>0</v>
+      </c>
+      <c r="N17" s="4">
+        <v>0</v>
+      </c>
+      <c r="O17" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" s="4">
+        <v>12000</v>
+      </c>
+      <c r="E18" s="4">
+        <v>6000</v>
+      </c>
+      <c r="F18" s="4">
+        <v>12000</v>
+      </c>
+      <c r="G18" s="4">
+        <v>6000</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L18" s="2">
+        <v>20</v>
+      </c>
+      <c r="M18" s="4">
+        <v>0</v>
+      </c>
+      <c r="N18" s="4">
+        <v>1</v>
+      </c>
+      <c r="O18" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="4">
+        <v>12000</v>
+      </c>
+      <c r="E19" s="4">
+        <v>6000</v>
+      </c>
+      <c r="F19" s="4">
+        <v>12000</v>
+      </c>
+      <c r="G19" s="4">
+        <v>6000</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L19" s="2">
+        <v>20</v>
+      </c>
+      <c r="M19" s="4">
+        <v>0</v>
+      </c>
+      <c r="N19" s="4">
+        <v>2</v>
+      </c>
+      <c r="O19" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="4">
+        <v>12000</v>
+      </c>
+      <c r="E20" s="4">
+        <v>6000</v>
+      </c>
+      <c r="F20" s="4">
+        <v>12000</v>
+      </c>
+      <c r="G20" s="4">
+        <v>6000</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L20" s="2">
+        <v>20</v>
+      </c>
+      <c r="M20" s="4">
+        <v>0</v>
+      </c>
+      <c r="N20" s="4">
+        <v>3</v>
+      </c>
+      <c r="O20" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="4">
+        <v>12000</v>
+      </c>
+      <c r="E21" s="4">
+        <v>6000</v>
+      </c>
+      <c r="F21" s="4">
+        <v>12000</v>
+      </c>
+      <c r="G21" s="4">
+        <v>6000</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L21" s="2">
+        <v>20</v>
+      </c>
+      <c r="M21" s="4">
+        <v>0</v>
+      </c>
+      <c r="N21" s="4">
+        <v>4</v>
+      </c>
+      <c r="O21" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="4">
+        <v>12000</v>
+      </c>
+      <c r="E22" s="4">
+        <v>6000</v>
+      </c>
+      <c r="F22" s="4">
+        <v>12000</v>
+      </c>
+      <c r="G22" s="4">
+        <v>6000</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L22" s="2">
+        <v>20</v>
+      </c>
+      <c r="M22" s="4">
+        <v>0</v>
+      </c>
+      <c r="N22" s="4">
+        <v>0</v>
+      </c>
+      <c r="O22" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" s="4">
+        <v>12000</v>
+      </c>
+      <c r="E23" s="4">
+        <v>6000</v>
+      </c>
+      <c r="F23" s="4">
+        <v>12000</v>
+      </c>
+      <c r="G23" s="4">
+        <v>6000</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L23" s="2">
+        <v>20</v>
+      </c>
+      <c r="M23" s="4">
+        <v>0</v>
+      </c>
+      <c r="N23" s="4">
+        <v>1</v>
+      </c>
+      <c r="O23" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" s="4">
+        <v>12000</v>
+      </c>
+      <c r="E24" s="4">
+        <v>6000</v>
+      </c>
+      <c r="F24" s="4">
+        <v>12000</v>
+      </c>
+      <c r="G24" s="4">
+        <v>6000</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L24" s="2">
+        <v>20</v>
+      </c>
+      <c r="M24" s="4">
+        <v>0</v>
+      </c>
+      <c r="N24" s="4">
+        <v>2</v>
+      </c>
+      <c r="O24" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" s="4">
+        <v>12000</v>
+      </c>
+      <c r="E25" s="4">
+        <v>6000</v>
+      </c>
+      <c r="F25" s="4">
+        <v>12000</v>
+      </c>
+      <c r="G25" s="4">
+        <v>6000</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L25" s="2">
+        <v>20</v>
+      </c>
+      <c r="M25" s="4">
+        <v>0</v>
+      </c>
+      <c r="N25" s="4">
+        <v>3</v>
+      </c>
+      <c r="O25" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" s="5"/>
+      <c r="C26" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" s="4">
+        <v>12000</v>
+      </c>
+      <c r="E26" s="4">
+        <v>6000</v>
+      </c>
+      <c r="F26" s="4">
+        <v>12000</v>
+      </c>
+      <c r="G26" s="4">
+        <v>6000</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L26" s="2">
+        <v>20</v>
+      </c>
+      <c r="M26" s="4">
+        <v>0</v>
+      </c>
+      <c r="N26" s="4">
+        <v>4</v>
+      </c>
+      <c r="O26" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27" s="4">
+        <v>12000</v>
+      </c>
+      <c r="E27" s="4">
+        <v>6000</v>
+      </c>
+      <c r="F27" s="4">
+        <v>12000</v>
+      </c>
+      <c r="G27" s="4">
+        <v>6000</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L27" s="2">
+        <v>20</v>
+      </c>
+      <c r="M27" s="4">
+        <v>0</v>
+      </c>
+      <c r="N27" s="4">
+        <v>0</v>
+      </c>
+      <c r="O27" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28" s="4">
+        <v>12000</v>
+      </c>
+      <c r="E28" s="4">
+        <v>6000</v>
+      </c>
+      <c r="F28" s="4">
+        <v>12000</v>
+      </c>
+      <c r="G28" s="4">
+        <v>6000</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L28" s="2">
+        <v>20</v>
+      </c>
+      <c r="M28" s="4">
+        <v>0</v>
+      </c>
+      <c r="N28" s="4">
+        <v>1</v>
+      </c>
+      <c r="O28" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" s="5"/>
+      <c r="C29" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D29" s="4">
+        <v>12000</v>
+      </c>
+      <c r="E29" s="4">
+        <v>6000</v>
+      </c>
+      <c r="F29" s="4">
+        <v>12000</v>
+      </c>
+      <c r="G29" s="4">
+        <v>6000</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L29" s="2">
+        <v>20</v>
+      </c>
+      <c r="M29" s="4">
+        <v>0</v>
+      </c>
+      <c r="N29" s="4">
+        <v>2</v>
+      </c>
+      <c r="O29" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30" s="5"/>
+      <c r="C30" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D30" s="4">
+        <v>12000</v>
+      </c>
+      <c r="E30" s="4">
+        <v>6000</v>
+      </c>
+      <c r="F30" s="4">
+        <v>12000</v>
+      </c>
+      <c r="G30" s="4">
+        <v>6000</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L30" s="2">
+        <v>20</v>
+      </c>
+      <c r="M30" s="4">
+        <v>0</v>
+      </c>
+      <c r="N30" s="4">
+        <v>3</v>
+      </c>
+      <c r="O30" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B31" s="5"/>
+      <c r="C31" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" s="4">
+        <v>12000</v>
+      </c>
+      <c r="E31" s="4">
+        <v>6000</v>
+      </c>
+      <c r="F31" s="4">
+        <v>12000</v>
+      </c>
+      <c r="G31" s="4">
+        <v>6000</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L31" s="2">
+        <v>20</v>
+      </c>
+      <c r="M31" s="4">
+        <v>0</v>
+      </c>
+      <c r="N31" s="4">
+        <v>4</v>
+      </c>
+      <c r="O31" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32" s="4">
+        <v>12000</v>
+      </c>
+      <c r="E32" s="4">
+        <v>6000</v>
+      </c>
+      <c r="F32" s="4">
+        <v>12000</v>
+      </c>
+      <c r="G32" s="4">
+        <v>6000</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K32" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L32" s="2">
+        <v>20</v>
+      </c>
+      <c r="M32" s="4">
+        <v>0</v>
+      </c>
+      <c r="N32" s="4">
+        <v>0</v>
+      </c>
+      <c r="O32" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33" s="4">
+        <v>12000</v>
+      </c>
+      <c r="E33" s="4">
+        <v>6000</v>
+      </c>
+      <c r="F33" s="4">
+        <v>12000</v>
+      </c>
+      <c r="G33" s="4">
+        <v>6000</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L33" s="2">
+        <v>20</v>
+      </c>
+      <c r="M33" s="4">
+        <v>0</v>
+      </c>
+      <c r="N33" s="4">
+        <v>1</v>
+      </c>
+      <c r="O33" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D34" s="4">
+        <v>12000</v>
+      </c>
+      <c r="E34" s="4">
+        <v>6000</v>
+      </c>
+      <c r="F34" s="4">
+        <v>12000</v>
+      </c>
+      <c r="G34" s="4">
+        <v>6000</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L34" s="2">
+        <v>20</v>
+      </c>
+      <c r="M34" s="4">
+        <v>0</v>
+      </c>
+      <c r="N34" s="4">
+        <v>2</v>
+      </c>
+      <c r="O34" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D35" s="4">
+        <v>12000</v>
+      </c>
+      <c r="E35" s="4">
+        <v>6000</v>
+      </c>
+      <c r="F35" s="4">
+        <v>12000</v>
+      </c>
+      <c r="G35" s="4">
+        <v>6000</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I35" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L35" s="2">
+        <v>20</v>
+      </c>
+      <c r="M35" s="4">
+        <v>0</v>
+      </c>
+      <c r="N35" s="4">
+        <v>3</v>
+      </c>
+      <c r="O35" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B36" s="6"/>
+      <c r="C36" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36" s="4">
+        <v>12000</v>
+      </c>
+      <c r="E36" s="4">
+        <v>6000</v>
+      </c>
+      <c r="F36" s="4">
+        <v>12000</v>
+      </c>
+      <c r="G36" s="4">
+        <v>6000</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L36" s="2">
+        <v>20</v>
+      </c>
+      <c r="M36" s="4">
+        <v>0</v>
+      </c>
+      <c r="N36" s="4">
+        <v>4</v>
+      </c>
+      <c r="O36" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat: added public comments to model; added new council mtgs to model; feat: tuned prompt
</commit_message>
<xml_diff>
--- a/packages/evaluate/gpt4.xlsx
+++ b/packages/evaluate/gpt4.xlsx
@@ -15,6 +15,7 @@
     <sheet name="test-1" sheetId="1" r:id="rId1"/>
     <sheet name="test-2" sheetId="2" r:id="rId2"/>
     <sheet name="test-3" sheetId="3" r:id="rId3"/>
+    <sheet name="test-4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="976" uniqueCount="118">
   <si>
     <t>what is city council doing to address racial inequality?</t>
   </si>
@@ -351,6 +352,45 @@
   </si>
   <si>
     <t>{"card_type": "in_depth", "responses": [{"response": "The transcripts show a complex picture of the New Orleans City Council's attitude towards the Mayor. There are instances of collaboration and support but also frustration and criticism."}, {"response": "On one hand, the council members acknowledge the Mayor's efforts. They mention his collaboration with the council to pass necessary legislation and his initiative to involve the council in task force meetings. The council also supports the Mayor's actions by approving ordinances that authorize him to enter into cooperative endeavor agreements with different agencies."}, {"response": "However, the transcripts also show instances of frustration with the Mayor's office. Members express dissatisfaction with the lack of clear leadership and communication from the administration, especially regarding city planning. They express frustration that the council was not involved in decisions that put the city's finances at risk. They also note that the council was not given an opportunity to participate or provide input regarding the legal strategy of some cases."}, {"response": "Overall, the transcripts show that while the council acknowledges the efforts of the Mayor, they also express frustration at times. There are instances of collaboration and support, but also a desire for better communication and inclusion in decision-making processes. However, the transcripts do not provide a clear consensus on whether the council thinks the Mayor is doing a good job."}], "citations": [{"Title": "City Council Meeting 1/5/23", "Published": "1/5/2023", "URL": "https://www.youtube.com/watch?v=bTR53b05t50&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "1:28:00-1:28:28", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 2-2-2023", "Published": "2/2/2023", "URL": "https://www.youtube.com/watch?v=Bl-Tv5yuUTw&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "3:37:59-3:38:24", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 1/5/23", "Published": "1/5/2023", "URL": "https://www.youtube.com/watch?v=bTR53b05t50&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "1:57:59-1:58:30", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 5/11/2023", "Published": "5/11/2023", "URL": "https://www.youtube.com/watch?v=ZX00_-VUSrM&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "5:02:12-5:02:39", "Name": "Regular City Council Meetings 2023.json"}]}</t>
+  </si>
+  <si>
+    <t>is NOPD's of FR effective according to quarterly reports</t>
+  </si>
+  <si>
+    <t>{"card_type": "in_depth", "responses": [{"response": "The New Orleans City Council has had its share of successes and challenges. "}, {"response": "A few successes include: "}, {"response": "1. The council amended the ordinance providing the operating budget of expenditures for the City of New Orleans for the year 2023. This allowed for an appropriation of funds to the office of cultural economic for business development, membership subscriptions, marketing, and events. "}, {"response": "2. They passed a resolution R23 167 encouraging the legislative auditor to conduct an audit of the sewage and water board of New Orleans, showing a commitment to maintaining checks and balances within the city's operations. "}, {"response": "3. The council successfully updated members as needed and engaged with their respective districts if the task force needed to be involved. "}, {"response": "4. They also managed to pass a resolution to authorize the president of the council to sign a loan agreement between the City of New Orleans and unity of Greater New Orleans East. "}, {"response": "However, there were also some challenges: "}, {"response": "1. One major challenge is that the council has been dealing with a systemic problem that neither they nor the school board can solve on their own. This highlights the difficulty of managing situations that fall within the purview of multiple entities. "}, {"response": "2. The council has struggled with addressing public safety issues, with mixed results from efforts to solve problems with the New Orleans Police Department as well as outsourcing to the New Orleans Police and Justice Foundation. "}, {"response": "3. There was also frustration expressed over the council's lack of involvement in decisions that affected the city's bottom line, particularly regarding lawsuits. "}, {"response": "4. The council also faced challenges in ensuring that the City of New Orleans got the return for the tremendous investment of taxes, fees, and fines. "}, {"response": "In conclusion, the council has shown a commitment to serving its community, passing important resolutions, and adjusting the city's budget. However, they have also struggled with challenges related to systemic problems, public safety, and legal strategy."}], "citations": [{"Title": "Regular City Council Meeting 4/20/2023", "Published": "4/20/2023", "URL": "https://www.youtube.com/watch?v=TUQ8MxcIWQI&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "5:23:04-5:23:28", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 2-2-2023", "Published": "2/2/2023", "URL": "https://www.youtube.com/watch?v=Bl-Tv5yuUTw&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "3:13:42-3:14:06", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 5/11/2023", "Published": "5/11/2023", "URL": "https://www.youtube.com/watch?v=ZX00_-VUSrM&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "4:53:57-4:54:22", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Criminal Justice Committee Meeting 4/5/2023", "Published": "4/5/2023", "URL": "https://www.youtube.com/watch?v=CRgme-Yh1yg&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "2:09:15-2:09:40", "Name": "Criminal Justice City Council Meeting Committee Meetings 2023.json"}, {"Title": "City Council Meeting 3/23/2023", "Published": "3/23/2023", "URL": "https://www.youtube.com/watch?v=xVZ-oOFqv70&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "1:39:16-1:39:41", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 3-9-2023", "Published": "3/9/2023", "URL": "https://www.youtube.com/watch?v=qTNPq_Gv5-E&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "50:48:00-51:19:00", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 5/11/2023", "Published": "5/11/2023", "URL": "https://www.youtube.com/watch?v=ZX00_-VUSrM&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "4:34:05-4:34:30", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Criminal Justice Committee Meeting 4/5/2023", "Published": "4/5/2023", "URL": "https://www.youtube.com/watch?v=CRgme-Yh1yg&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "11:32-12:02", "Name": "Criminal Justice City Council Meeting Committee Meetings 2023.json"}, {"Title": "Regular City Council Meeting 4/20/2023", "Published": "4/20/2023", "URL": "https://www.youtube.com/watch?v=TUQ8MxcIWQI&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "3:49:00-3:49:22", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 1/5/23", "Published": "1/5/2023", "URL": "https://www.youtube.com/watch?v=bTR53b05t50&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "1:30:15-1:30:42", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 1/5/23", "Published": "1/5/2023", "URL": "https://www.youtube.com/watch?v=bTR53b05t50&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "1:28:00-1:28:28", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Regular City Council Meeting 4/20/2023", "Published": "4/20/2023", "URL": "https://www.youtube.com/watch?v=TUQ8MxcIWQI&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "5:12:19-5:12:44", "Name": "Regular City Council Meetings 2023.json"}]}</t>
+  </si>
+  <si>
+    <t>{"card_type": "in_depth", "responses": [{"response": "The New Orleans City Council has seen both successes and failures in its operations and decisions. "}, {"response": "In terms of successes, the council has been proactive in addressing mental health issues among the youth. This is evident in the amendment to the Cooperative Endeavor agreement between the city and the Children's Bureau of New Orleans, which extended the agreement for an additional year and increased the maximum aggregate amount of compensation. This initiative demonstrates the council's commitment to ensuring the well-being of the city's young population. "}, {"response": "The council has also shown a commitment to improving the living standards of the city's workers. They have authorized the mayor to enter into an agreement to provide wage enhancements for child care workers, waived requirements regarding residency, and raised pay for various positions. "}, {"response": "The council has also taken steps to address issues of code violation and blight, as well as supporting strategic economic development plans and beautification projects in various communities. "}, {"response": "However, the council has also faced criticism and challenges. One major issue has been the sharp increase in short-term rentals, which some believe has contributed to a rise in rent prices and has turned affordable housing into accommodations for tourists. This shift has reportedly exacerbated the city's housing crisis, with many residents unable to afford homes and struggling with neglected rental units."}, {"response": "Another criticism is the council's alleged lack of investment in the city's youth, with claims that only 3% of the city's budget is allocated to supporting young people. The council has also been criticized for not involving the public in decisions that put the city's bottom line at risk."}, {"response": "There are also concerns about the council's decision to change zoning from multi-family housing to single-family housing, which some argue limits the amount of housing available to citizens. "}, {"response": "In conclusion, while the council has made strides in areas such as mental health services for youth and wage enhancement for workers, it has also faced criticism for its handling of the housing crisis and its perceived lack of investment in the city's youth."}], "citations": [{"Title": "City Council Meeting 6/8/2023", "Published": "6/8/2023", "URL": "https://www.youtube.com/watch?v=XDMh4kiWRnM&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "1:45:48-1:46:17", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Regular Council Meeting", "Published": "6/8/2023", "URL": "https://www.youtube.com/watch?v=XDMh4kiWRnM", "Video timestamp": "1:45:48-1:46:17", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Regular Council Meeting", "Published": "7/27/2023", "URL": "https://www.youtube.com/watch?v=gSft2c7mAhE", "Video timestamp": "3:41:30-3:41:57", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 3/23/2023", "Published": "3/23/2023", "URL": "https://www.youtube.com/watch?v=xVZ-oOFqv70&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "4:24:46-4:25:08", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Regular Council Meeting", "Published": "7/27/2023", "URL": "https://www.youtube.com/watch?v=gSft2c7mAhE", "Video timestamp": "4:34:56-4:35:20", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 6/8/2023", "Published": "6/8/2023", "URL": "https://www.youtube.com/watch?v=XDMh4kiWRnM&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "2:04:16-2:04:41", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Regular Council Meeting", "Published": "7/27/2023", "URL": "https://www.youtube.com/watch?v=gSft2c7mAhE", "Video timestamp": "3:53:11-3:53:39", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 3/23/2023", "Published": "3/23/2023", "URL": "https://www.youtube.com/watch?v=xVZ-oOFqv70&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "7:39:17-7:39:41", "Name": "Regular City Council Meetings 2023.json"}]}</t>
+  </si>
+  <si>
+    <t>{"card_type": "in_depth", "responses": [{"response": "Based on the transcripts, the New Orleans City Council has had both successes and failures in its endeavors."}, {"response": "Successes of the city council include passing various resolutions and ordinances. For example, resolution R23 343 was passed unanimously, which reaffirms the council's commitment to the safety and quality of life for all citizens, including transgender and gender non-conforming individuals. The council also passed a resolution stating they would not increase sewage and water board rates until the utility demonstrates it has implemented all aspects pointed out by the local director of council relations. "}, {"response": "Moreover, the council authorized the mayor to enter into a cooperative agreement with the Odyssey House and worked on affordable housing development. Council members also expressed unity in their goal of providing affordable housing in New Orleans, marking another success."}, {"response": "However, there were also failures and criticisms. Some council members were criticized for repeatedly proposing the use of increased surveillance and facial recognition, which some constituents opposed due to privacy concerns. It was suggested that these proposals were ineffective solutions to crime and that the council should focus more on addressing lack of resources, enduring trauma, and improving the social safety net. "}, {"response": "Another failure noted was in relation to the council's handling of renter protection. One comment criticized the council for not acting urgently enough to protect renters from homelessness, abuse, and exploitation from slumlords. It was suggested the council should focus on creating healthy homes as soon as possible."}, {"response": "There was also criticism of the council for allegedly misusing funds. The council was accused of continuously allocating money into the New Orleans Police Department, which was then allegedly used to illegally purchase vehicles. "}, {"response": "In conclusion, the New Orleans City Council has had successes in passing resolutions and working towards affordable housing, but has also faced criticism and failures related to surveillance proposals, renter's protections, and alleged misuse of funds."}], "citations": [{"Title": "Regular Council Meeting", "Published": "7/27/2023", "URL": "https://www.youtube.com/watch?v=gSft2c7mAhE", "Video timestamp": "4:20:14-4:20:38", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 5/11/2023", "Published": "5/11/2023", "URL": "https://www.youtube.com/watch?v=ZX00_-VUSrM&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "5:34:44-5:35:13", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Regular Council Meeting", "Published": "7/13/2023", "URL": "https://www.youtube.com/watch?v=39kWL1P9NoI", "Video timestamp": "3:00:33-3:00:57", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 1/5/23", "Published": "1/5/2023", "URL": "https://www.youtube.com/watch?v=bTR53b05t50&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "2:29:56-2:30:32", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 5/11/2023", "Published": "5/11/2023", "URL": "https://www.youtube.com/watch?v=ZX00_-VUSrM&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "5:02:12-5:02:39", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 3/23/2023", "Published": "3/23/2023", "URL": "https://www.youtube.com/watch?v=xVZ-oOFqv70&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "1:38:45-1:39:11", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Regular City Council Meeting 7/21/2023", "Published": "7/21/2023", "Name": "Regular City Council Meeting 7-21-2022.json"}]}</t>
+  </si>
+  <si>
+    <t>{"card_type": "in_depth", "responses": [{"response": "The New Orleans City Council has had both success and failures, as is typical in any governing body. "}, {"response": "On the positive side, the council has made efforts to address the needs of the community. For example, they have passed ordinances to provide funds for rental assistance programs and to assist homeowners in addressing code enforcement violations. The council has also worked to amend budgets to provide for necessary expenditures such as personnel overtime for the police department and the purchase of security systems equipment and software. They have also sought to ensure public safety and community development. For instance, one of the resolutions urged the New Orleans mayor to conduct a national search for a new police superintendent, with a focus on inclusive, transparent, and clearly defined public processes. "}, {"response": "However, there have been criticisms of the council's actions as well. For example, the council has faced backlash for considering an ordinance related to surveillance technologies. Critics argue that the council cannot guarantee safety, accountability, or oversight with these tools and that the ordinance could lead to increased repression and potential abuse. There is also concern about the council's handling of allegations of misconduct related to the NOLA Coalition\u2019s involvement in pushing for this ordinance, with accusations of manipulation and misuse of private funds. "}, {"response": "The council has also received criticism for its handling of police matters. There have been complaints about the NOPD's corruption and abuse, and accusations that the council is negligent for considering giving them more access to potentially dangerous tools and technologies. Despite these criticisms, the council has made efforts to solve these issues, such as outsourcing to the New Orleans Police and Justice Foundation, although the results have been less than satisfactory according to the critics. "}, {"response": "In summary, while the New Orleans City Council has had successes in legislating for community needs and public safety, they have also faced challenges and criticisms, particularly around issues of surveillance and policing."}], "citations": [{"Title": "Regular City Council Meeting 7/21/2023", "Published": "7/21/2023", "Name": "Regular City Council Meeting 7-21-2022.json"}, {"Title": "Regular Council Meeting", "Published": "6/8/2023", "URL": "https://www.youtube.com/watch?v=XDMh4kiWRnM", "Video timestamp": "4:31:54-4:32:26", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 6/8/2023", "Published": "6/8/2023", "URL": "https://www.youtube.com/watch?v=XDMh4kiWRnM&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "4:31:54-4:32:26", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Regular Council Meeting", "Published": "7/27/2023", "URL": "https://www.youtube.com/watch?v=gSft2c7mAhE", "Video timestamp": "3:59:04-3:59:30", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 1/5/23", "Published": "1/5/2023", "URL": "https://www.youtube.com/watch?v=bTR53b05t50&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "2:39:24-2:39:50", "Name": "Regular City Council Meetings 2023.json"}]}</t>
+  </si>
+  <si>
+    <t>{"card_type": "in_depth", "responses": [{"response": "Based on the transcripts, the city council members mentioned are:"}, {"response": "1. Council member Thomas\n2. Council member Morrell\n3. Council member Moreno\n4. Council member King\n5. Council member Harris\n6. Council member Jeruso\n7. Council member Green"}, {"response": "Please note that the transcripts do not provide any additional information about these council members, such as their district or specific roles within the council beyond the mentions of council member Morrell being elected as president and council member Moreno being elected as vice president."}], "citations": [{"Title": "Criminal Justice Committee Meeting", "Published": "12/14/2022", "URL": "https://www.youtube.com/watch?v=fxbVwYjIaok&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "7:16-7:40", "Name": "Criminal Justice City Council Meeting Committee Meetings 2023.json"}, {"Title": "City Council Meeting 3-9-2023", "Published": "3/9/2023", "URL": "https://www.youtube.com/watch?v=qTNPq_Gv5-E&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "5:17:00-5:17:27", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Regular Council Meeting", "Published": "7/27/2023", "URL": "https://www.youtube.com/watch?v=gSft2c7mAhE", "Video timestamp": "56:31:00-57:55:00", "Name": "Regular City Council Meetings 2023.json"}]}</t>
+  </si>
+  <si>
+    <t>{"card_type": "in_depth", "responses": [{"response": "The transcript does not provide specific descriptions for each individual city council member. It does, however, highlight several council members and their roles or actions within the council, as follows:"}, {"response": "1. Council Member Thomas: He is mentioned expressing gratitude for the work done by others and emphasizing the importance of providing opportunities for young people."}, {"response": "2. Council Member Harris: He is recognized for his efforts in acknowledging someone who has dedicated their life to creating opportunities for young people. He also provided an opportunity for Devin Wright to present to the Quality of Life Committee, showing his involvement in sustainability and environmental discussions."}, {"response": "3. Council Member Green: He is associated with a PSA about the greatness of New Orleans as a place to work. He is also recognized for understanding the difficulties of the issues the council is dealing with."}, {"response": "4. Council Member Jeruso: He is identified as the budget chair and is praised for his leadership. He is also involved in amending ordinances related to the city's budget and workforce development."}, {"response": "5. Council Member Moreno: She is elected to serve as the vice president of the council for the term starting January 5th, 2023."}, {"response": "6. Council Member Morrell: He is elected to serve as the president of the council for the term starting January 5th, 2023."}, {"response": "7. Council Member King: While not described individually, he is listed as one of the council members."}, {"response": "It is important to note that this summary is based on the specific actions and roles mentioned in the transcript, and does not cover the entirety of each council member's duties or contributions."}], "citations": [{"Title": "Criminal Justice Committee Meeting 5/10/2023", "Published": "5/10/2023", "URL": "https://www.youtube.com/watch?v=kqfTCmIlvjw&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "2:12:50-2:13:14", "Name": "Criminal Justice City Council Meeting Committee Meetings 2023.json"}, {"Title": "City Council Meeting 3-9-2023", "Published": "3/9/2023", "URL": "https://www.youtube.com/watch?v=qTNPq_Gv5-E&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "50:48:00-51:19:00", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 3-9-2023", "Published": "3/9/2023", "URL": "https://www.youtube.com/watch?v=qTNPq_Gv5-E&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "4:30:08-4:30:34", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 1/5/23", "Published": "1/5/2023", "URL": "https://www.youtube.com/watch?v=bTR53b05t50&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "2:39:24-2:39:50", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Regular City Council Meeting 4/20/2023", "Published": "4/20/2023", "URL": "https://www.youtube.com/watch?v=TUQ8MxcIWQI&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "5:19:19-5:19:44", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 1/5/23", "Published": "1/5/2023", "URL": "https://www.youtube.com/watch?v=bTR53b05t50&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "1:28:00-1:28:28", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Criminal Justice Committee Meeting 4/5/2023", "Published": "4/5/2023", "URL": "https://www.youtube.com/watch?v=CRgme-Yh1yg&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "2:09:15-2:09:40", "Name": "Criminal Justice City Council Meeting Committee Meetings 2023.json"}, {"Title": "Regular Council Meeting", "Published": "7/13/2023", "URL": "https://www.youtube.com/watch?v=39kWL1P9NoI", "Video timestamp": "3:35:18-3:35:43", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 6/8/2023", "Published": "6/8/2023", "URL": "https://www.youtube.com/watch?v=XDMh4kiWRnM&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "1:32:37-1:33:00", "Name": "Regular City Council Meetings 2023.json"}]}</t>
+  </si>
+  <si>
+    <t>{"card_type": "in_depth", "responses": [{"response": "The New Orleans City Council has undertaken a number of actions to address racial inequality, many of which involve legislation aimed at creating affordable housing and resisting harmful surveillance practices that disproportionately affect communities of color."}, {"response": "In the transcripts, we see that council members Harris, Moreno, and King have directed the City Planning Commission to conduct public hearings to consider amendments to the comprehensive zoning ordinance. These amendments aim to create standards for affordable home ownership opportunities, which could help address systemic racial inequalities in home ownership and wealth accumulation."}, {"response": "Council member Harris also moved for an ordinance to amend the operating budget to appropriate funds for rental assistance programs and a pilot program to assist homeowners in addressing code enforcement violations. This could help to mitigate some of the effects of historic racial and economic inequality."}, {"response": "The Council has also been vocal in opposing the implementation of racially biased surveillance technology. Many speakers at the Council's meetings have criticized the use of surveillance technology, particularly facial recognition, arguing that it disproportionately targets and falsely identifies people of color. In response to these concerns, the Council passed Ordinance 33021 in December 2020 to safeguard residents against the city's use of harmful surveillance tools. There is, however, controversy over proposed Ordinance 33639, which some argue could roll back these protections."}, {"response": "The Council also passed Resolution R23 199, reaffirming its commitment to the safety and equality of all citizens, including transgender and gender non-conforming individuals."}, {"response": "In summary, the City Council has taken steps to address racial inequality in New Orleans through zoning amendments, budget allocations, and legislation aimed at protecting citizens from harmful surveillance practices. However, the transcripts also reveal ongoing debates and differing perspectives on these issues."}], "citations": [{"Title": "Regular City Council Meeting 7/21/2023", "Published": "7/21/2023", "Name": "Regular City Council Meeting 7-21-2022.json"}, {"Title": "City Council Meeting 3/23/2023", "Published": "3/23/2023", "URL": "https://www.youtube.com/watch?v=xVZ-oOFqv70&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "7:12:11-7:12:40", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Smart and Sustainable Cities Committee Meeting 7/8/2022", "Published": "7/8/2022", "Name": "Smart and Sustainable Cities Committee Meeting 7-8-2022.json"}, {"Title": "City Council Meeting 1-19-2023", "Published": "1/19/2023", "URL": "https://www.youtube.com/watch?v=7Nro7f26oEo&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "4:40:59-4:41:30", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 1-19-2023", "Published": "1/19/2023", "URL": "https://www.youtube.com/watch?v=7Nro7f26oEo&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "3:25:48-3:26:19", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Criminal Justice Committee Meeting 4/5/2023", "Published": "4/5/2023", "URL": "https://www.youtube.com/watch?v=CRgme-Yh1yg&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "19:49-20:15", "Name": "Criminal Justice City Council Meeting Committee Meetings 2023.json"}]}</t>
+  </si>
+  <si>
+    <t>{"card_type": "in_depth", "responses": [{"response": "The New Orleans City Council is addressing racial inequality through various measures. One of the ways is through the passage of Ordinance 33021 in December 2020, which bans the use of facial recognition software. This technology has been proven to be susceptible to error and misidentification, particularly in communities of color and on marginalized citizens. The ordinance gives the City Council the ability to review all future surveillance technologies adopted by the city, allowing them to regulate technology that could disproportionately impact communities of color. "}, {"response": "However, there is concern that Mayor Cantrell and Chief of Police Shaun Ferguson are trying to reverse this ordinance, which has led to some criticism from the public. The council is urged to maintain the ban on this technology and to prioritize other issues such as affordable housing, healthcare, utility bills, debt, un-liveable wages, and trauma from hurricanes and pandemics. "}, {"response": "The City Council is also taking steps to address racial inequality by allocating funds for various programs. For instance, an ordinance has been proposed to appropriate funds to The Orleans Parish Public Defender's office within miscellaneous programs for criminal defense representation to indigent persons accused of committing crimes in New Orleans Parish. Moreover, there's a proposal to appropriate unspent funds to the Department of Workforce Development."}, {"response": "While the council is taking measures to address racial inequality, some residents feel more could be done, particularly in the areas of workers' rights, public transport, and creating and maintaining jobs that pay a living wage. There are also calls for the council to resist the incorporation of racially biased surveillance technology as part of its crime-prevention strategy and to focus instead on addressing the root causes of crime. "}, {"response": "In summary, the New Orleans City Council is making efforts to address racial inequality, but there is ongoing debate about the effectiveness and focus of these measures."}], "citations": [{"Title": "City Council Meeting 3/23/2023", "Published": "3/23/2023", "URL": "https://www.youtube.com/watch?v=xVZ-oOFqv70&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "2:10:11-2:10:36", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Regular Council Meeting", "Published": "7/13/2023", "URL": "https://www.youtube.com/watch?v=39kWL1P9NoI", "Video timestamp": "3:35:18-3:35:43", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Smart and Sustainable Cities Committee Meeting 7/8/2022", "Published": "7/8/2022", "Name": "Smart and Sustainable Cities Committee Meeting 7-8-2022.json"}, {"Title": "Regular Council Meeting", "Published": "7/13/2023", "URL": "https://www.youtube.com/watch?v=39kWL1P9NoI", "Video timestamp": "3:00:33-3:00:57", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Regular City Council Meeting 7/21/2023", "Published": "7/21/2023", "Name": "Regular City Council Meeting 7-21-2022.json"}]}</t>
+  </si>
+  <si>
+    <t>{"card_type": "in_depth", "responses": [{"response": "An ordinance, in the context of the New Orleans City Council, is a piece of legislation or law enacted by the city council. It is a formal rule or law that the council creates and enforces to regulate various aspects of the city's operations, community safety, and public affairs. "}, {"response": "In the process of making an ordinance, it is first considered at a committee meeting and then laid over for at least 20 days. Any amendment to the ordinance by a non-authoring council member must be received by the author and council member at least 48 hours in advance of the council meeting at which the ordinance will be considered. "}, {"response": "Ordinances can cover a wide range of issues, from public safety to zoning regulations. For instance, council members may introduce an ordinance to amend the city code to increase the default penalty for violations, revoke the dedication to public use for community safety reasons, or establish an exemption for contracts approved by ordinance."}, {"response": "The council also has the power to consider and vote on amendments to an ordinance. These amendments must be germane to the instrument's original purpose and cannot alter or nullify the original purpose of the ordinance."}, {"response": "Once an ordinance is adopted, it becomes law and is enforced within the city. The adoption of an ordinance often requires a majority vote from the council members. The Lakeview Civic Improvement Association (LCIA), for example, asked for a deferral on voting on a specific ordinance until the public had enough time to review and assess its implications. "}, {"response": "In summary, an ordinance is a piece of legislation passed by the city council that regulates various aspects of city life, and its creation, amendment, and adoption involve a detailed democratic process."}], "citations": [{"Title": "City Council Meeting 6/8/2023", "Published": "6/8/2023", "URL": "https://www.youtube.com/watch?v=XDMh4kiWRnM&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "3:34:16-3:34:42", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Regular Council Meeting", "Published": "7/27/2023", "URL": "https://www.youtube.com/watch?v=gSft2c7mAhE", "Video timestamp": "3:25:35-3:26:02", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Regular Council Meeting", "Published": "7/27/2023", "URL": "https://www.youtube.com/watch?v=gSft2c7mAhE", "Video timestamp": "3:51:31-3:52:01", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Smart and Sustainable Cities Committee Meeting 7/8/2022", "Published": "7/8/2022", "Name": "Smart and Sustainable Cities Committee Meeting 7-8-2022.json"}, {"Title": "City Council Meeting 6/8/2023", "Published": "6/8/2023", "URL": "https://www.youtube.com/watch?v=XDMh4kiWRnM&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "3:31:50-3:32:14", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Regular Council Meeting", "Published": "6/8/2023", "URL": "https://www.youtube.com/watch?v=XDMh4kiWRnM", "Video timestamp": "3:31:50-3:32:14", "Name": "Regular City Council Meetings 2023.json"}]}</t>
+  </si>
+  <si>
+    <t>{"card_type": "in_depth", "responses": [{"response": "An ordinance, as referenced in the New Orleans City Council transcripts, is a piece of legislation enacted by a local government, such as a city or county. These pieces of legislation are often used to regulate a wide variety of activities to protect and maintain the peace, safety, and welfare of the community. "}, {"response": "In the context of the transcripts, ordinances are being used to establish and amend various rules, regulations, and programs within the City of New Orleans. Examples include the program to assist homeowners in addressing code enforcement violations and historical district landmarks commission, appropriating funds for rental assistance programs, and reviewing security technologies before they are implemented to maintain transparency. "}, {"response": "Ordinances are also used to authorize agreements, such as the First Amendment to a previously executed Cooperative Endeavor agreement between the City of New Orleans and the New Orleans Redevelopment Authority as mentioned in the transcript. "}, {"response": "The transcripts also refer to amendments being made to existing ordinances. These amendments can be technical in nature or can significantly impact the ordinance's content. When an ordinance is amended, the wording is adjusted, and the changes are voted on by council members. "}, {"response": "The council members play a significant role in the creation, amendment, and approval of these ordinances. They are the ones who propose and discuss the details of these pieces of legislation, and they vote on whether or not to implement them. Their decisions are based on the needs and welfare of the community they represent. "}, {"response": "The transcripts also mention the enforcement of these ordinances, emphasizing the importance of ensuring that the rules and regulations established by these ordinances are followed, and that any violations are appropriately addressed. "}, {"response": "The process of passing an ordinance includes several steps, such as introduction, committee review, public hearing, and council vote. If approved, the ordinance becomes law and is enforced within the jurisdiction of the local government. "}, {"response": "In conclusion, an ordinance in the context of the New Orleans City Council transcripts is a form of legislation that helps regulate and govern various aspects of the city's operations, services, and community standards. It is a vital tool for local government to maintain order, provide services, and protect the welfare of their constituents."}], "citations": [{"Title": "City Council Meeting 6/8/2023", "Published": "6/8/2023", "URL": "https://www.youtube.com/watch?v=XDMh4kiWRnM&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "4:31:54-4:32:26", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Regular Council Meeting", "Published": "6/8/2023", "URL": "https://www.youtube.com/watch?v=XDMh4kiWRnM", "Video timestamp": "4:31:54-4:32:26", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 3/23/2023", "Published": "3/23/2023", "URL": "https://www.youtube.com/watch?v=xVZ-oOFqv70&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "2:59:19-2:59:52", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Regular Council Meeting", "Published": "7/27/2023", "URL": "https://www.youtube.com/watch?v=gSft2c7mAhE", "Video timestamp": "3:26:09-3:26:34", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Smart and Sustainable Cities Committee Meeting 7/8/2022", "Published": "7/8/2022", "Name": "Smart and Sustainable Cities Committee Meeting 7-8-2022.json"}, {"Title": "City Council Meeting 3/23/2023", "Published": "3/23/2023", "URL": "https://www.youtube.com/watch?v=xVZ-oOFqv70&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "7:28:03-7:28:26", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Regular Council Meeting", "Published": "7/27/2023", "URL": "https://www.youtube.com/watch?v=gSft2c7mAhE", "Video timestamp": "3:51:31-3:52:01", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Smart and Sustainable Cities Committee Meeting 7/8/2022", "Published": "7/8/2022", "Name": "Smart and Sustainable Cities Committee Meeting 7-8-2022.json"}]}</t>
+  </si>
+  <si>
+    <t>{"card_type": "in_depth", "responses": [{"response": "The transcripts do not provide explicit statements from the city council members about their opinion on the performance of the mayor. However, there are several indications that they appreciate the collaborative efforts between the council and the mayor's office."}, {"response": "For instance, one council member acknowledges that \"the mayor worked in tandem with city council and got the legislation necessary to put things in motion to get them done.\" This suggests an appreciation for the mayor's collaborative efforts and ability to get things done. Similarly, another council member expressed gratitude for the mayor's efforts in supporting the New Orleans Police Department, which could imply a positive view of the mayor's work."}, {"response": "However, there are also instances in the transcript where the council members express dissatisfaction with certain issues in the city, such as the pay of the chief of police and the issue of homelessness. While these concerns are raised, they are not directly attributed to the mayor's performance."}, {"response": "Overall, based on the transcripts, it appears that the city council members generally appreciate the collaborative efforts between the mayor's office and the city council, but they also express concerns about specific issues in the city. However, without explicit statements about the mayor's performance, it is not possible to definitively conclude whether they think the mayor is doing a good job."}], "citations": [{"Title": "City Council Meeting 5/11/2023", "Published": "5/11/2023", "URL": "https://www.youtube.com/watch?v=ZX00_-VUSrM&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "26:28:00-26:54:00", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Criminal Justice Committee Meeting", "Published": "7/12/2023", "URL": "https://www.youtube.com/watch?v=dsO7iShH97E", "Video timestamp": "1:06:10-1:06:34", "Name": "Criminal Justice City Council Meeting Committee Meetings 2023.json"}, {"Title": "City Council Meeting 6/8/2023", "Published": "6/8/2023", "URL": "https://www.youtube.com/watch?v=XDMh4kiWRnM&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "4:19:05-4:19:32", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "Regular Council Meeting", "Published": "6/8/2023", "URL": "https://www.youtube.com/watch?v=XDMh4kiWRnM", "Video timestamp": "4:19:05-4:19:32", "Name": "Regular City Council Meetings 2023.json"}]}</t>
+  </si>
+  <si>
+    <t>{"card_type": "in_depth", "responses": [{"response": "The transcripts do not provide a clear, direct assessment of the Mayor's performance from the perspective of the city council. However, there are mentions of collaborative work between the Mayor and the city council, which suggest a degree of cooperation and shared goals. For instance, there is a mention of the Mayor working in tandem with the city council to get necessary legislation in motion and ensuring that matters were attended to properly. There's also a reference to the Mayor encouraging the entire New Orleans city council to participate in any committee meetings held by the task force. "}, {"response": "On the other hand, there's a hint of some disagreement or differing opinions, as one council member mentions that they had \"a previous mayor and a present mayor who said they didn't favor\" something, without specifying what that something is. "}, {"response": "Overall, it's clear that the city council appreciates collaboration with the Mayor's office, but without more context or specific commentary, it's difficult to definitively determine the council's overall opinion on the Mayor's performance."}], "citations": [{"Title": "Criminal Justice Committee Meeting 4/5/2023", "Published": "4/5/2023", "URL": "https://www.youtube.com/watch?v=CRgme-Yh1yg&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "2:07:15-2:07:39", "Name": "Criminal Justice City Council Meeting Committee Meetings 2023.json"}, {"Title": "Regular City Council Meeting 4/20/2023", "Published": "4/20/2023", "URL": "https://www.youtube.com/watch?v=TUQ8MxcIWQI&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "39:06:00-39:31:00", "Name": "Regular City Council Meetings 2023.json"}, {"Title": "City Council Meeting 1/5/23", "Published": "1/5/2023", "URL": "https://www.youtube.com/watch?v=bTR53b05t50&amp;ab_channel=NewOrleansCityCouncil", "Video timestamp": "2:42:55-2:43:20", "Name": "Regular City Council Meetings 2023.json"}]}</t>
   </si>
 </sst>
 </file>
@@ -1959,8 +1999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O31"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection sqref="A1:O31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3432,8 +3472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="O33" sqref="O33"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3492,21 +3532,45 @@
       <c r="B2" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="4">
+        <v>12000</v>
+      </c>
+      <c r="E2" s="4">
+        <v>6000</v>
+      </c>
+      <c r="F2" s="4">
+        <v>12000</v>
+      </c>
+      <c r="G2" s="4">
+        <v>6000</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="L2" s="2">
         <v>20</v>
       </c>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="3"/>
+      <c r="M2" s="4">
+        <v>0</v>
+      </c>
+      <c r="N2" s="4">
+        <v>0</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
@@ -3515,21 +3579,45 @@
       <c r="B3" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
+      <c r="C3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="4">
+        <v>12000</v>
+      </c>
+      <c r="E3" s="4">
+        <v>6000</v>
+      </c>
+      <c r="F3" s="4">
+        <v>12000</v>
+      </c>
+      <c r="G3" s="4">
+        <v>6000</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="L3" s="2">
         <v>20</v>
       </c>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="3"/>
+      <c r="M3" s="4">
+        <v>0</v>
+      </c>
+      <c r="N3" s="4">
+        <v>0</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="4" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
@@ -3538,21 +3626,45 @@
       <c r="B4" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
+      <c r="C4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="4">
+        <v>12000</v>
+      </c>
+      <c r="E4" s="4">
+        <v>6000</v>
+      </c>
+      <c r="F4" s="4">
+        <v>12000</v>
+      </c>
+      <c r="G4" s="4">
+        <v>6000</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="L4" s="2">
         <v>20</v>
       </c>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="3"/>
+      <c r="M4" s="4">
+        <v>0</v>
+      </c>
+      <c r="N4" s="4">
+        <v>0</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="5" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
@@ -3561,21 +3673,45 @@
       <c r="B5" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
+      <c r="C5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="4">
+        <v>12000</v>
+      </c>
+      <c r="E5" s="4">
+        <v>6000</v>
+      </c>
+      <c r="F5" s="4">
+        <v>12000</v>
+      </c>
+      <c r="G5" s="4">
+        <v>6000</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="L5" s="2">
         <v>20</v>
       </c>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="3"/>
+      <c r="M5" s="4">
+        <v>0</v>
+      </c>
+      <c r="N5" s="4">
+        <v>0</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="6" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
@@ -3584,21 +3720,45 @@
       <c r="B6" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
+      <c r="C6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="4">
+        <v>12000</v>
+      </c>
+      <c r="E6" s="4">
+        <v>6000</v>
+      </c>
+      <c r="F6" s="4">
+        <v>12000</v>
+      </c>
+      <c r="G6" s="4">
+        <v>6000</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="L6" s="2">
         <v>20</v>
       </c>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="3"/>
+      <c r="M6" s="4">
+        <v>0</v>
+      </c>
+      <c r="N6" s="4">
+        <v>0</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="7" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
@@ -4960,6 +5120,1665 @@
       </c>
       <c r="G36" s="4">
         <v>6000</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L36" s="2">
+        <v>20</v>
+      </c>
+      <c r="M36" s="4">
+        <v>0</v>
+      </c>
+      <c r="N36" s="4">
+        <v>4</v>
+      </c>
+      <c r="O36" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O36"/>
+  <sheetViews>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2">
+        <v>20000</v>
+      </c>
+      <c r="E2" s="2">
+        <v>10000</v>
+      </c>
+      <c r="F2" s="2">
+        <v>20000</v>
+      </c>
+      <c r="G2" s="2">
+        <v>10000</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L2" s="2">
+        <v>20</v>
+      </c>
+      <c r="M2" s="4">
+        <v>0</v>
+      </c>
+      <c r="N2" s="4">
+        <v>0</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2">
+        <v>20000</v>
+      </c>
+      <c r="E3" s="2">
+        <v>10000</v>
+      </c>
+      <c r="F3" s="2">
+        <v>20000</v>
+      </c>
+      <c r="G3" s="2">
+        <v>10000</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L3" s="2">
+        <v>20</v>
+      </c>
+      <c r="M3" s="4">
+        <v>0</v>
+      </c>
+      <c r="N3" s="4">
+        <v>0</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="2">
+        <v>20000</v>
+      </c>
+      <c r="E4" s="2">
+        <v>10000</v>
+      </c>
+      <c r="F4" s="2">
+        <v>20000</v>
+      </c>
+      <c r="G4" s="2">
+        <v>10000</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L4" s="2">
+        <v>20</v>
+      </c>
+      <c r="M4" s="4">
+        <v>0</v>
+      </c>
+      <c r="N4" s="4">
+        <v>0</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2">
+        <v>20000</v>
+      </c>
+      <c r="E5" s="2">
+        <v>10000</v>
+      </c>
+      <c r="F5" s="2">
+        <v>20000</v>
+      </c>
+      <c r="G5" s="2">
+        <v>10000</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L5" s="2">
+        <v>20</v>
+      </c>
+      <c r="M5" s="4">
+        <v>0</v>
+      </c>
+      <c r="N5" s="4">
+        <v>0</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="2">
+        <v>20000</v>
+      </c>
+      <c r="E6" s="2">
+        <v>10000</v>
+      </c>
+      <c r="F6" s="2">
+        <v>20000</v>
+      </c>
+      <c r="G6" s="2">
+        <v>10000</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L6" s="2">
+        <v>20</v>
+      </c>
+      <c r="M6" s="4">
+        <v>0</v>
+      </c>
+      <c r="N6" s="4">
+        <v>0</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="2">
+        <v>20000</v>
+      </c>
+      <c r="E7" s="2">
+        <v>10000</v>
+      </c>
+      <c r="F7" s="2">
+        <v>20000</v>
+      </c>
+      <c r="G7" s="2">
+        <v>10000</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L7" s="2">
+        <v>20</v>
+      </c>
+      <c r="M7" s="4">
+        <v>0</v>
+      </c>
+      <c r="N7" s="4">
+        <v>0</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="2">
+        <v>20000</v>
+      </c>
+      <c r="E8" s="2">
+        <v>10000</v>
+      </c>
+      <c r="F8" s="2">
+        <v>20000</v>
+      </c>
+      <c r="G8" s="2">
+        <v>10000</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L8" s="2">
+        <v>20</v>
+      </c>
+      <c r="M8" s="4">
+        <v>0</v>
+      </c>
+      <c r="N8" s="4">
+        <v>0</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="2">
+        <v>20000</v>
+      </c>
+      <c r="E9" s="2">
+        <v>10000</v>
+      </c>
+      <c r="F9" s="2">
+        <v>20000</v>
+      </c>
+      <c r="G9" s="2">
+        <v>10000</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L9" s="2">
+        <v>20</v>
+      </c>
+      <c r="M9" s="4">
+        <v>0</v>
+      </c>
+      <c r="N9" s="4">
+        <v>0</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="2">
+        <v>20000</v>
+      </c>
+      <c r="E10" s="2">
+        <v>10000</v>
+      </c>
+      <c r="F10" s="2">
+        <v>20000</v>
+      </c>
+      <c r="G10" s="2">
+        <v>10000</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L10" s="2">
+        <v>20</v>
+      </c>
+      <c r="M10" s="4">
+        <v>0</v>
+      </c>
+      <c r="N10" s="4">
+        <v>0</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="2">
+        <v>20000</v>
+      </c>
+      <c r="E11" s="2">
+        <v>10000</v>
+      </c>
+      <c r="F11" s="2">
+        <v>20000</v>
+      </c>
+      <c r="G11" s="2">
+        <v>10000</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L11" s="2">
+        <v>20</v>
+      </c>
+      <c r="M11" s="4">
+        <v>0</v>
+      </c>
+      <c r="N11" s="4">
+        <v>0</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" s="2">
+        <v>20000</v>
+      </c>
+      <c r="E12" s="2">
+        <v>10000</v>
+      </c>
+      <c r="F12" s="2">
+        <v>20000</v>
+      </c>
+      <c r="G12" s="2">
+        <v>10000</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L12" s="2">
+        <v>20</v>
+      </c>
+      <c r="M12" s="4">
+        <v>0</v>
+      </c>
+      <c r="N12" s="4">
+        <v>0</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="2">
+        <v>20000</v>
+      </c>
+      <c r="E13" s="2">
+        <v>10000</v>
+      </c>
+      <c r="F13" s="2">
+        <v>20000</v>
+      </c>
+      <c r="G13" s="2">
+        <v>10000</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L13" s="2">
+        <v>20</v>
+      </c>
+      <c r="M13" s="4">
+        <v>0</v>
+      </c>
+      <c r="N13" s="4">
+        <v>1</v>
+      </c>
+      <c r="O13" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="2">
+        <v>20000</v>
+      </c>
+      <c r="E14" s="2">
+        <v>10000</v>
+      </c>
+      <c r="F14" s="2">
+        <v>20000</v>
+      </c>
+      <c r="G14" s="2">
+        <v>10000</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L14" s="2">
+        <v>20</v>
+      </c>
+      <c r="M14" s="4">
+        <v>0</v>
+      </c>
+      <c r="N14" s="4">
+        <v>2</v>
+      </c>
+      <c r="O14" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="2">
+        <v>20000</v>
+      </c>
+      <c r="E15" s="2">
+        <v>10000</v>
+      </c>
+      <c r="F15" s="2">
+        <v>20000</v>
+      </c>
+      <c r="G15" s="2">
+        <v>10000</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L15" s="2">
+        <v>20</v>
+      </c>
+      <c r="M15" s="4">
+        <v>0</v>
+      </c>
+      <c r="N15" s="4">
+        <v>3</v>
+      </c>
+      <c r="O15" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="2">
+        <v>20000</v>
+      </c>
+      <c r="E16" s="2">
+        <v>10000</v>
+      </c>
+      <c r="F16" s="2">
+        <v>20000</v>
+      </c>
+      <c r="G16" s="2">
+        <v>10000</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L16" s="2">
+        <v>20</v>
+      </c>
+      <c r="M16" s="4">
+        <v>0</v>
+      </c>
+      <c r="N16" s="4">
+        <v>4</v>
+      </c>
+      <c r="O16" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="2">
+        <v>20000</v>
+      </c>
+      <c r="E17" s="2">
+        <v>10000</v>
+      </c>
+      <c r="F17" s="2">
+        <v>20000</v>
+      </c>
+      <c r="G17" s="2">
+        <v>10000</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L17" s="2">
+        <v>20</v>
+      </c>
+      <c r="M17" s="4">
+        <v>0</v>
+      </c>
+      <c r="N17" s="4">
+        <v>0</v>
+      </c>
+      <c r="O17" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D18" s="2">
+        <v>20000</v>
+      </c>
+      <c r="E18" s="2">
+        <v>10000</v>
+      </c>
+      <c r="F18" s="2">
+        <v>20000</v>
+      </c>
+      <c r="G18" s="2">
+        <v>10000</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L18" s="2">
+        <v>20</v>
+      </c>
+      <c r="M18" s="4">
+        <v>0</v>
+      </c>
+      <c r="N18" s="4">
+        <v>1</v>
+      </c>
+      <c r="O18" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="2">
+        <v>20000</v>
+      </c>
+      <c r="E19" s="2">
+        <v>10000</v>
+      </c>
+      <c r="F19" s="2">
+        <v>20000</v>
+      </c>
+      <c r="G19" s="2">
+        <v>10000</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L19" s="2">
+        <v>20</v>
+      </c>
+      <c r="M19" s="4">
+        <v>0</v>
+      </c>
+      <c r="N19" s="4">
+        <v>2</v>
+      </c>
+      <c r="O19" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" s="2">
+        <v>20000</v>
+      </c>
+      <c r="E20" s="2">
+        <v>10000</v>
+      </c>
+      <c r="F20" s="2">
+        <v>20000</v>
+      </c>
+      <c r="G20" s="2">
+        <v>10000</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L20" s="2">
+        <v>20</v>
+      </c>
+      <c r="M20" s="4">
+        <v>0</v>
+      </c>
+      <c r="N20" s="4">
+        <v>3</v>
+      </c>
+      <c r="O20" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="2">
+        <v>20000</v>
+      </c>
+      <c r="E21" s="2">
+        <v>10000</v>
+      </c>
+      <c r="F21" s="2">
+        <v>20000</v>
+      </c>
+      <c r="G21" s="2">
+        <v>10000</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L21" s="2">
+        <v>20</v>
+      </c>
+      <c r="M21" s="4">
+        <v>0</v>
+      </c>
+      <c r="N21" s="4">
+        <v>4</v>
+      </c>
+      <c r="O21" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="5"/>
+      <c r="C22" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="2">
+        <v>20000</v>
+      </c>
+      <c r="E22" s="2">
+        <v>10000</v>
+      </c>
+      <c r="F22" s="2">
+        <v>20000</v>
+      </c>
+      <c r="G22" s="2">
+        <v>10000</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L22" s="2">
+        <v>20</v>
+      </c>
+      <c r="M22" s="4">
+        <v>0</v>
+      </c>
+      <c r="N22" s="4">
+        <v>0</v>
+      </c>
+      <c r="O22" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="5"/>
+      <c r="C23" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" s="2">
+        <v>20000</v>
+      </c>
+      <c r="E23" s="2">
+        <v>10000</v>
+      </c>
+      <c r="F23" s="2">
+        <v>20000</v>
+      </c>
+      <c r="G23" s="2">
+        <v>10000</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L23" s="2">
+        <v>20</v>
+      </c>
+      <c r="M23" s="4">
+        <v>0</v>
+      </c>
+      <c r="N23" s="4">
+        <v>1</v>
+      </c>
+      <c r="O23" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="5"/>
+      <c r="C24" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" s="2">
+        <v>20000</v>
+      </c>
+      <c r="E24" s="2">
+        <v>10000</v>
+      </c>
+      <c r="F24" s="2">
+        <v>20000</v>
+      </c>
+      <c r="G24" s="2">
+        <v>10000</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L24" s="2">
+        <v>20</v>
+      </c>
+      <c r="M24" s="4">
+        <v>0</v>
+      </c>
+      <c r="N24" s="4">
+        <v>2</v>
+      </c>
+      <c r="O24" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" s="2">
+        <v>20000</v>
+      </c>
+      <c r="E25" s="2">
+        <v>10000</v>
+      </c>
+      <c r="F25" s="2">
+        <v>20000</v>
+      </c>
+      <c r="G25" s="2">
+        <v>10000</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L25" s="2">
+        <v>20</v>
+      </c>
+      <c r="M25" s="4">
+        <v>0</v>
+      </c>
+      <c r="N25" s="4">
+        <v>3</v>
+      </c>
+      <c r="O25" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="5"/>
+      <c r="C26" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" s="2">
+        <v>20000</v>
+      </c>
+      <c r="E26" s="2">
+        <v>10000</v>
+      </c>
+      <c r="F26" s="2">
+        <v>20000</v>
+      </c>
+      <c r="G26" s="2">
+        <v>10000</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L26" s="2">
+        <v>20</v>
+      </c>
+      <c r="M26" s="4">
+        <v>0</v>
+      </c>
+      <c r="N26" s="4">
+        <v>4</v>
+      </c>
+      <c r="O26" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27" s="2">
+        <v>20000</v>
+      </c>
+      <c r="E27" s="2">
+        <v>10000</v>
+      </c>
+      <c r="F27" s="2">
+        <v>20000</v>
+      </c>
+      <c r="G27" s="2">
+        <v>10000</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L27" s="2">
+        <v>20</v>
+      </c>
+      <c r="M27" s="4">
+        <v>0</v>
+      </c>
+      <c r="N27" s="4">
+        <v>0</v>
+      </c>
+      <c r="O27" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28" s="2">
+        <v>20000</v>
+      </c>
+      <c r="E28" s="2">
+        <v>10000</v>
+      </c>
+      <c r="F28" s="2">
+        <v>20000</v>
+      </c>
+      <c r="G28" s="2">
+        <v>10000</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L28" s="2">
+        <v>20</v>
+      </c>
+      <c r="M28" s="4">
+        <v>0</v>
+      </c>
+      <c r="N28" s="4">
+        <v>1</v>
+      </c>
+      <c r="O28" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D29" s="2">
+        <v>20000</v>
+      </c>
+      <c r="E29" s="2">
+        <v>10000</v>
+      </c>
+      <c r="F29" s="2">
+        <v>20000</v>
+      </c>
+      <c r="G29" s="2">
+        <v>10000</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L29" s="2">
+        <v>20</v>
+      </c>
+      <c r="M29" s="4">
+        <v>0</v>
+      </c>
+      <c r="N29" s="4">
+        <v>2</v>
+      </c>
+      <c r="O29" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B30" s="5"/>
+      <c r="C30" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D30" s="2">
+        <v>20000</v>
+      </c>
+      <c r="E30" s="2">
+        <v>10000</v>
+      </c>
+      <c r="F30" s="2">
+        <v>20000</v>
+      </c>
+      <c r="G30" s="2">
+        <v>10000</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L30" s="2">
+        <v>20</v>
+      </c>
+      <c r="M30" s="4">
+        <v>0</v>
+      </c>
+      <c r="N30" s="4">
+        <v>3</v>
+      </c>
+      <c r="O30" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" s="5"/>
+      <c r="C31" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" s="2">
+        <v>20000</v>
+      </c>
+      <c r="E31" s="2">
+        <v>10000</v>
+      </c>
+      <c r="F31" s="2">
+        <v>20000</v>
+      </c>
+      <c r="G31" s="2">
+        <v>10000</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L31" s="2">
+        <v>20</v>
+      </c>
+      <c r="M31" s="4">
+        <v>0</v>
+      </c>
+      <c r="N31" s="4">
+        <v>4</v>
+      </c>
+      <c r="O31" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32" s="2">
+        <v>20000</v>
+      </c>
+      <c r="E32" s="2">
+        <v>10000</v>
+      </c>
+      <c r="F32" s="2">
+        <v>20000</v>
+      </c>
+      <c r="G32" s="2">
+        <v>10000</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K32" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L32" s="2">
+        <v>20</v>
+      </c>
+      <c r="M32" s="4">
+        <v>0</v>
+      </c>
+      <c r="N32" s="4">
+        <v>0</v>
+      </c>
+      <c r="O32" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33" s="2">
+        <v>20000</v>
+      </c>
+      <c r="E33" s="2">
+        <v>10000</v>
+      </c>
+      <c r="F33" s="2">
+        <v>20000</v>
+      </c>
+      <c r="G33" s="2">
+        <v>10000</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L33" s="2">
+        <v>20</v>
+      </c>
+      <c r="M33" s="4">
+        <v>0</v>
+      </c>
+      <c r="N33" s="4">
+        <v>1</v>
+      </c>
+      <c r="O33" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" s="6"/>
+      <c r="C34" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D34" s="2">
+        <v>20000</v>
+      </c>
+      <c r="E34" s="2">
+        <v>10000</v>
+      </c>
+      <c r="F34" s="2">
+        <v>20000</v>
+      </c>
+      <c r="G34" s="2">
+        <v>10000</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L34" s="2">
+        <v>20</v>
+      </c>
+      <c r="M34" s="4">
+        <v>0</v>
+      </c>
+      <c r="N34" s="4">
+        <v>2</v>
+      </c>
+      <c r="O34" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D35" s="2">
+        <v>20000</v>
+      </c>
+      <c r="E35" s="2">
+        <v>10000</v>
+      </c>
+      <c r="F35" s="2">
+        <v>20000</v>
+      </c>
+      <c r="G35" s="2">
+        <v>10000</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I35" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="L35" s="2">
+        <v>20</v>
+      </c>
+      <c r="M35" s="4">
+        <v>0</v>
+      </c>
+      <c r="N35" s="4">
+        <v>3</v>
+      </c>
+      <c r="O35" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B36" s="6"/>
+      <c r="C36" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36" s="2">
+        <v>20000</v>
+      </c>
+      <c r="E36" s="2">
+        <v>10000</v>
+      </c>
+      <c r="F36" s="2">
+        <v>20000</v>
+      </c>
+      <c r="G36" s="2">
+        <v>10000</v>
       </c>
       <c r="H36" s="4" t="s">
         <v>48</v>

</xml_diff>